<commit_message>
finished stacked design, annotaded
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
+++ b/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10076C2D-F6EA-4A92-8436-5CC08967089F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13198BC6-8EBC-4816-A345-6974DA9DA442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,21 +16,21 @@
     <sheet name="2ndMainBoard" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$64</definedName>
     <definedName name="Z_14407C96_79A3_4D80_86DC_7BE14F8182CE_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$I:$I,'2ndMainBoard'!$M:$M,'2ndMainBoard'!$P:$R,'2ndMainBoard'!$T:$AD</definedName>
-    <definedName name="Z_14407C96_79A3_4D80_86DC_7BE14F8182CE_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$62</definedName>
+    <definedName name="Z_14407C96_79A3_4D80_86DC_7BE14F8182CE_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$64</definedName>
     <definedName name="Z_86D49B71_F0A7_4EDF_9F83_437E8F1DE26F_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$H:$L,'2ndMainBoard'!$Q:$R,'2ndMainBoard'!$T:$U</definedName>
-    <definedName name="Z_86D49B71_F0A7_4EDF_9F83_437E8F1DE26F_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$62</definedName>
+    <definedName name="Z_86D49B71_F0A7_4EDF_9F83_437E8F1DE26F_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$64</definedName>
     <definedName name="Z_AD0CFDC5_A886_4774_8323_B873BC9D36B7_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$F:$L,'2ndMainBoard'!$Q:$R,'2ndMainBoard'!$T:$V</definedName>
-    <definedName name="Z_AD0CFDC5_A886_4774_8323_B873BC9D36B7_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$62</definedName>
-    <definedName name="Z_E3E09E1D_E21B_434F_8777_BA2F5DFE998D_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$62</definedName>
+    <definedName name="Z_AD0CFDC5_A886_4774_8323_B873BC9D36B7_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$64</definedName>
+    <definedName name="Z_E3E09E1D_E21B_434F_8777_BA2F5DFE998D_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
     <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
-    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="309">
   <si>
     <t>Alternative</t>
   </si>
@@ -688,9 +688,6 @@
     <t>44A0221-16-9/9CS3030</t>
   </si>
   <si>
-    <t>USB-C Stecker</t>
-  </si>
-  <si>
     <t>Schutzschlatung</t>
   </si>
   <si>
@@ -962,6 +959,48 @@
   </si>
   <si>
     <t>5V</t>
+  </si>
+  <si>
+    <t>Ferritperle</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/tdk-corporation/MPZ1005S331ET000/3910121</t>
+  </si>
+  <si>
+    <t>MPZ1005S331ET000</t>
+  </si>
+  <si>
+    <t>330 Ω @ 100 MHz, 0,5 Ω DC, 700mA</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>USB-C Kabel</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/assmann-wsw-components/A-USB31C-20A-150A/10408414</t>
+  </si>
+  <si>
+    <t>A-USB31C-20A-150A</t>
+  </si>
+  <si>
+    <t>22 AWG, 28 AWG, USB 2.0, 1.5m</t>
+  </si>
+  <si>
+    <t>USB-C Buchse</t>
+  </si>
+  <si>
+    <t>TD-103-T-A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/de/products/detail/samtec-inc/TD-103-T-A/1105555</t>
+  </si>
+  <si>
+    <t>TS-103-T-A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/de/products/detail/samtec-inc/TS-103-T-A/1105491</t>
   </si>
 </sst>
 </file>
@@ -1948,11 +1987,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AD93"/>
+  <dimension ref="A1:AD95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2041,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>122</v>
@@ -2017,13 +2056,13 @@
         <v>7</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L1" s="23" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N1" s="24" t="s">
         <v>9</v>
@@ -2044,14 +2083,14 @@
         <v>14</v>
       </c>
       <c r="U1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X1" s="60" t="s">
         <v>106</v>
       </c>
       <c r="Y1" s="61"/>
       <c r="Z1" s="11">
-        <f>SUMIFS(P10:P62,Q10:Q62, "Nicht Gekauft",R10:R62,"Benötigt")</f>
+        <f>SUMIFS(P10:P64,Q10:Q64, "Nicht Gekauft",R10:R64,"Benötigt")</f>
         <v>64.3</v>
       </c>
       <c r="AB1" s="58" t="s">
@@ -2059,8 +2098,8 @@
       </c>
       <c r="AC1" s="59"/>
       <c r="AD1" s="10">
-        <f>SUM(P2:P62)</f>
-        <v>391.23999999999995</v>
+        <f>SUM(P2:P64)</f>
+        <v>400.78999999999996</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -2099,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="32">
-        <f t="shared" ref="P2:P62" si="0">N2*O2</f>
+        <f t="shared" ref="P2:P64" si="0">N2*O2</f>
         <v>9.91</v>
       </c>
       <c r="Q2" s="33" t="s">
@@ -2149,7 +2188,7 @@
         <v>27</v>
       </c>
       <c r="M3" s="31" t="str">
-        <f t="shared" ref="M3:M62" si="1">HYPERLINK(L3,J3)</f>
+        <f t="shared" ref="M3:M64" si="1">HYPERLINK(L3,J3)</f>
         <v>AZ-Delivery</v>
       </c>
       <c r="N3" s="40">
@@ -2169,7 +2208,7 @@
         <v>109</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U62" si="2">SUBTOTAL(103, G3)</f>
+        <f t="shared" ref="U3:U64" si="2">SUBTOTAL(103, G3)</f>
         <v>1</v>
       </c>
     </row>
@@ -2289,25 +2328,25 @@
       </c>
       <c r="Y5" s="65"/>
       <c r="Z5" s="12">
-        <f>SUBTOTAL(9,P1:P62)</f>
-        <v>197.02</v>
+        <f>SUBTOTAL(9,P1:P64)</f>
+        <v>202.76000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>269</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>270</v>
       </c>
       <c r="C6" s="36" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="35" t="s">
         <v>272</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>273</v>
       </c>
       <c r="F6" s="35">
         <v>0.5</v>
@@ -2322,7 +2361,7 @@
       </c>
       <c r="K6" s="38"/>
       <c r="L6" s="39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="40">
@@ -2407,7 +2446,7 @@
       </c>
       <c r="Y7" s="63"/>
       <c r="Z7" s="9">
-        <f>SUBTOTAL(9,T1:T62)</f>
+        <f>SUBTOTAL(9,T1:T64)</f>
         <v>30.18</v>
       </c>
     </row>
@@ -2708,7 +2747,7 @@
       </c>
       <c r="K13" s="42"/>
       <c r="L13" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M13" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2764,7 +2803,7 @@
       </c>
       <c r="K14" s="36"/>
       <c r="L14" s="39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M14" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2812,7 +2851,7 @@
       </c>
       <c r="K15" s="42"/>
       <c r="L15" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M15" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2994,16 +3033,16 @@
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="28" t="s">
-        <v>204</v>
+        <v>304</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>87</v>
       </c>
       <c r="D19" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>215</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>216</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
@@ -3014,7 +3053,7 @@
       </c>
       <c r="K19" s="42"/>
       <c r="L19" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M19" s="31" t="str">
         <f t="shared" si="1"/>
@@ -3370,7 +3409,8 @@
       <c r="O26" s="41">
         <v>10</v>
       </c>
-      <c r="P26" s="40">
+      <c r="P26" s="32">
+        <f>N26*O26</f>
         <v>1</v>
       </c>
       <c r="Q26" s="37"/>
@@ -3429,487 +3469,481 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35" t="s">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="B28" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" s="42"/>
+      <c r="L28" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="M28" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>DigiKey</v>
+      </c>
+      <c r="N28" s="32">
+        <v>9.25</v>
+      </c>
+      <c r="O28" s="33">
+        <v>1</v>
+      </c>
+      <c r="P28" s="32">
+        <f>N28*O28</f>
+        <v>9.25</v>
+      </c>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C29" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D29" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="36" t="s">
+      <c r="E29" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38" t="s">
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="K28" s="38"/>
-      <c r="L28" s="39" t="s">
+      <c r="K29" s="38"/>
+      <c r="L29" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="M28" s="31" t="str">
+      <c r="M29" s="31" t="str">
         <f t="shared" si="1"/>
         <v>Amazon</v>
       </c>
-      <c r="N28" s="40">
+      <c r="N29" s="40">
         <v>8.66</v>
       </c>
-      <c r="O28" s="41">
+      <c r="O29" s="41">
         <v>1</v>
       </c>
-      <c r="P28" s="40">
+      <c r="P29" s="40">
         <f t="shared" si="0"/>
         <v>8.66</v>
       </c>
-      <c r="Q28" s="41" t="s">
+      <c r="Q29" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="R28" s="25" t="s">
+      <c r="R29" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="T28">
-        <f>IF(AND(Q28="Nicht Gekauft", R28="Benötigt"), P28, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="U28">
+      <c r="T29">
+        <f>IF(AND(Q29="Nicht Gekauft", R29="Benötigt"), P29, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28" t="s">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C30" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D30" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E30" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42" t="s">
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K29" s="42"/>
-      <c r="L29" s="31" t="s">
-        <v>262</v>
-      </c>
-      <c r="M29" s="31" t="str">
+      <c r="K30" s="42"/>
+      <c r="L30" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="M30" s="31" t="str">
         <f t="shared" si="1"/>
         <v>Amazon</v>
       </c>
-      <c r="N29" s="32">
+      <c r="N30" s="32">
         <v>5.99</v>
       </c>
-      <c r="O29" s="33">
+      <c r="O30" s="33">
         <v>1</v>
       </c>
-      <c r="P29" s="32">
+      <c r="P30" s="32">
         <f t="shared" si="0"/>
         <v>5.99</v>
       </c>
-      <c r="Q29" s="33" t="s">
+      <c r="Q30" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="R29" s="34" t="s">
+      <c r="R30" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="T29">
-        <f>IF(AND(Q29="Nicht Gekauft", R29="Benötigt"), P29, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="U29">
+      <c r="T30">
+        <f>IF(AND(Q30="Nicht Gekauft", R30="Benötigt"), P30, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U30">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="35" t="s">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="35"/>
+      <c r="B31" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C31" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D31" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E31" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36" t="s">
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="K30" s="36"/>
-      <c r="L30" s="39" t="s">
-        <v>262</v>
-      </c>
-      <c r="M30" s="31" t="str">
+      <c r="K31" s="36"/>
+      <c r="L31" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="M31" s="31" t="str">
         <f t="shared" si="1"/>
         <v>Amazon</v>
       </c>
-      <c r="N30" s="40">
+      <c r="N31" s="40">
         <v>18.14</v>
       </c>
-      <c r="O30" s="41">
+      <c r="O31" s="41">
         <v>1</v>
       </c>
-      <c r="P30" s="40">
+      <c r="P31" s="40">
         <f t="shared" si="0"/>
         <v>18.14</v>
       </c>
-      <c r="Q30" s="41" t="s">
+      <c r="Q31" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="R30" s="25" t="s">
+      <c r="R31" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="T30">
-        <f>IF(AND(Q30="Nicht Gekauft", R30="Benötigt"), P30, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="K31" s="42"/>
-      <c r="L31" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="M31" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>DigiKey</v>
-      </c>
-      <c r="N31" s="32">
-        <v>2.91</v>
-      </c>
-      <c r="O31" s="33">
-        <v>2</v>
-      </c>
-      <c r="P31" s="32">
-        <f t="shared" ref="P31:P43" si="6">N31*O31</f>
-        <v>5.82</v>
-      </c>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="34"/>
+      <c r="T31">
+        <f>IF(AND(Q31="Nicht Gekauft", R31="Benötigt"), P31, 0)</f>
+        <v>0</v>
+      </c>
       <c r="U31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="35" t="s">
-        <v>251</v>
-      </c>
-      <c r="C32" s="36" t="s">
+      <c r="A32" s="28"/>
+      <c r="B32" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="D32" s="37" t="s">
-        <v>252</v>
-      </c>
-      <c r="E32" s="35" t="s">
-        <v>253</v>
-      </c>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36" t="s">
+      <c r="C32" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="36"/>
-      <c r="L32" s="39" t="s">
-        <v>254</v>
+      <c r="K32" s="42"/>
+      <c r="L32" s="31" t="s">
+        <v>234</v>
       </c>
       <c r="M32" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
-      <c r="N32" s="40">
-        <v>0.41</v>
-      </c>
-      <c r="O32" s="41">
-        <v>1</v>
-      </c>
-      <c r="P32" s="40">
-        <f>N32*O32</f>
-        <v>0.41</v>
-      </c>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="25"/>
+      <c r="N32" s="32">
+        <v>2.91</v>
+      </c>
+      <c r="O32" s="33">
+        <v>2</v>
+      </c>
+      <c r="P32" s="32">
+        <f t="shared" ref="P32:P45" si="6">N32*O32</f>
+        <v>5.82</v>
+      </c>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="34"/>
       <c r="U32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42" t="s">
+      <c r="A33" s="35"/>
+      <c r="B33" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="K33" s="42"/>
-      <c r="L33" s="31" t="s">
-        <v>256</v>
+      <c r="K33" s="36"/>
+      <c r="L33" s="39" t="s">
+        <v>253</v>
       </c>
       <c r="M33" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
-      <c r="N33" s="32">
-        <v>0.23</v>
-      </c>
-      <c r="O33" s="33">
+      <c r="N33" s="40">
+        <v>0.41</v>
+      </c>
+      <c r="O33" s="41">
         <v>1</v>
       </c>
-      <c r="P33" s="32">
+      <c r="P33" s="40">
         <f>N33*O33</f>
-        <v>0.23</v>
-      </c>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="34"/>
+        <v>0.41</v>
+      </c>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="25"/>
       <c r="U33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="35" t="s">
-        <v>229</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="D34" s="35" t="s">
-        <v>231</v>
-      </c>
-      <c r="E34" s="35" t="s">
+      <c r="A34" s="28"/>
+      <c r="B34" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="C34" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36" t="s">
+      <c r="D34" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K34" s="36"/>
-      <c r="L34" s="39" t="s">
-        <v>230</v>
+      <c r="K34" s="42"/>
+      <c r="L34" s="31" t="s">
+        <v>255</v>
       </c>
       <c r="M34" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
-      <c r="N34" s="40">
-        <v>1.56</v>
-      </c>
-      <c r="O34" s="41">
+      <c r="N34" s="32">
+        <v>0.23</v>
+      </c>
+      <c r="O34" s="33">
         <v>1</v>
       </c>
-      <c r="P34" s="40">
+      <c r="P34" s="32">
         <f>N34*O34</f>
-        <v>1.56</v>
-      </c>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="25"/>
+        <v>0.23</v>
+      </c>
+      <c r="Q34" s="33"/>
+      <c r="R34" s="34"/>
       <c r="U34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28" t="s">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="35"/>
+      <c r="B35" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35" s="36"/>
+      <c r="L35" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="M35" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>DigiKey</v>
+      </c>
+      <c r="N35" s="40">
+        <v>1.56</v>
+      </c>
+      <c r="O35" s="41">
+        <v>1</v>
+      </c>
+      <c r="P35" s="40">
+        <f>N35*O35</f>
+        <v>1.56</v>
+      </c>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="25"/>
+      <c r="U35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K36" s="42"/>
+      <c r="L36" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="C35" s="42" t="s">
-        <v>205</v>
-      </c>
-      <c r="D35" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="K35" s="42"/>
-      <c r="L35" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="M35" s="31" t="str">
+      <c r="M36" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
-      <c r="N35" s="32">
+      <c r="N36" s="32">
         <v>0.47</v>
       </c>
-      <c r="O35" s="33">
+      <c r="O36" s="33">
         <v>1</v>
       </c>
-      <c r="P35" s="32">
+      <c r="P36" s="32">
         <f t="shared" si="6"/>
         <v>0.47</v>
       </c>
-      <c r="Q35" s="33"/>
-      <c r="R35" s="34"/>
-      <c r="U35">
+      <c r="Q36" s="33"/>
+      <c r="R36" s="34"/>
+      <c r="U36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="35" t="s">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="35">
+        <v>824521241</v>
+      </c>
+      <c r="E37" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="K37" s="36"/>
+      <c r="L37" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="D36" s="35">
-        <v>824521241</v>
-      </c>
-      <c r="E36" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="K36" s="36"/>
-      <c r="L36" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="M36" s="31" t="str">
+      <c r="M37" s="31" t="str">
         <f t="shared" si="1"/>
         <v>Digikey</v>
       </c>
-      <c r="N36" s="40">
+      <c r="N37" s="40">
         <v>0.3</v>
       </c>
-      <c r="O36" s="41">
+      <c r="O37" s="41">
         <v>1</v>
       </c>
-      <c r="P36" s="40">
+      <c r="P37" s="40">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="25"/>
-      <c r="U36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="K37" s="42"/>
-      <c r="L37" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="M37" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>DigiKey</v>
-      </c>
-      <c r="N37" s="32">
-        <v>5.79</v>
-      </c>
-      <c r="O37" s="33">
-        <v>1</v>
-      </c>
-      <c r="P37" s="32">
-        <f>N37*O37</f>
-        <v>5.79</v>
-      </c>
-      <c r="Q37" s="33"/>
-      <c r="R37" s="34"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="25"/>
       <c r="U37">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3917,19 +3951,19 @@
     </row>
     <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>247</v>
+        <v>295</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
       <c r="E38" s="35" t="s">
-        <v>249</v>
+        <v>298</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="35"/>
@@ -3940,51 +3974,40 @@
       </c>
       <c r="K38" s="36"/>
       <c r="L38" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="M38" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>DigiKey</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="M38" s="31"/>
       <c r="N38" s="40">
-        <v>4.1399999999999997</v>
+        <v>0.3</v>
       </c>
       <c r="O38" s="41">
         <v>1</v>
       </c>
       <c r="P38" s="40">
-        <f>N38*O38</f>
-        <v>4.1399999999999997</v>
+        <f t="shared" si="6"/>
+        <v>0.3</v>
       </c>
       <c r="Q38" s="41"/>
       <c r="R38" s="25"/>
-      <c r="U38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C39" s="42" t="s">
         <v>45</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>285</v>
+        <v>243</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="F39" s="28">
-        <v>0.05</v>
-      </c>
-      <c r="G39" s="28">
-        <v>5</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="42"/>
       <c r="J39" s="42" t="s">
@@ -3992,40 +4015,44 @@
       </c>
       <c r="K39" s="42"/>
       <c r="L39" s="31" t="s">
-        <v>284</v>
+        <v>244</v>
       </c>
       <c r="M39" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N39" s="32">
-        <v>2.34</v>
+        <v>5.79</v>
       </c>
       <c r="O39" s="33">
         <v>1</v>
       </c>
-      <c r="P39" s="40">
-        <f t="shared" ref="P39:P40" si="7">N39*O39</f>
-        <v>2.34</v>
+      <c r="P39" s="32">
+        <f>N39*O39</f>
+        <v>5.79</v>
       </c>
       <c r="Q39" s="33"/>
       <c r="R39" s="34"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C40" s="36" t="s">
         <v>45</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
@@ -4036,41 +4063,47 @@
       </c>
       <c r="K40" s="36"/>
       <c r="L40" s="39" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
       <c r="M40" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N40" s="40">
-        <v>1.17</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="O40" s="41">
         <v>1</v>
       </c>
       <c r="P40" s="40">
-        <f t="shared" si="7"/>
-        <v>1.17</v>
+        <f>N40*O40</f>
+        <v>4.1399999999999997</v>
       </c>
       <c r="Q40" s="41"/>
       <c r="R40" s="25"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
+      <c r="U40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
+        <v>282</v>
+      </c>
       <c r="B41" s="28" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="C41" s="42" t="s">
         <v>45</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="F41" s="28">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="G41" s="28">
         <v>5</v>
@@ -4082,49 +4115,43 @@
       </c>
       <c r="K41" s="42"/>
       <c r="L41" s="31" t="s">
-        <v>213</v>
+        <v>283</v>
       </c>
       <c r="M41" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N41" s="32">
-        <v>2.5499999999999998</v>
+        <v>2.34</v>
       </c>
       <c r="O41" s="33">
         <v>1</v>
       </c>
-      <c r="P41" s="32">
-        <f t="shared" si="6"/>
-        <v>2.5499999999999998</v>
+      <c r="P41" s="40">
+        <f t="shared" ref="P41:P42" si="7">N41*O41</f>
+        <v>2.34</v>
       </c>
       <c r="Q41" s="33"/>
       <c r="R41" s="34"/>
-      <c r="U41">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+    </row>
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="35" t="s">
+        <v>282</v>
+      </c>
       <c r="B42" s="35" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>219</v>
+        <v>287</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="F42" s="35">
-        <v>0.04</v>
-      </c>
-      <c r="G42" s="35">
-        <v>5</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
       <c r="H42" s="35"/>
       <c r="I42" s="36"/>
       <c r="J42" s="36" t="s">
@@ -4132,42 +4159,38 @@
       </c>
       <c r="K42" s="36"/>
       <c r="L42" s="39" t="s">
-        <v>218</v>
+        <v>286</v>
       </c>
       <c r="M42" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N42" s="40">
-        <v>4.5999999999999996</v>
+        <v>1.17</v>
       </c>
       <c r="O42" s="41">
         <v>1</v>
       </c>
       <c r="P42" s="40">
-        <f t="shared" si="6"/>
-        <v>4.5999999999999996</v>
+        <f t="shared" si="7"/>
+        <v>1.17</v>
       </c>
       <c r="Q42" s="41"/>
       <c r="R42" s="25"/>
-      <c r="U42">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="28" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C43" s="42" t="s">
         <v>45</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F43" s="28">
         <v>0.02</v>
@@ -4182,21 +4205,21 @@
       </c>
       <c r="K43" s="42"/>
       <c r="L43" s="31" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="M43" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N43" s="32">
-        <v>0.6</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="O43" s="33">
         <v>1</v>
       </c>
       <c r="P43" s="32">
         <f t="shared" si="6"/>
-        <v>0.6</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="Q43" s="33"/>
       <c r="R43" s="34"/>
@@ -4208,126 +4231,116 @@
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>34</v>
+        <v>216</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>45</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>31</v>
+        <v>218</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
+        <v>219</v>
+      </c>
+      <c r="F44" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="G44" s="35">
+        <v>5</v>
+      </c>
       <c r="H44" s="35"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="38" t="s">
+      <c r="I44" s="36"/>
+      <c r="J44" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="K44" s="38"/>
+      <c r="K44" s="36"/>
       <c r="L44" s="39" t="s">
-        <v>37</v>
+        <v>217</v>
       </c>
       <c r="M44" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N44" s="40">
-        <v>0.88</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="O44" s="41">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P44" s="40">
-        <f t="shared" si="0"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="Q44" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="R44" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="S44" s="6"/>
-      <c r="T44">
-        <f t="shared" ref="T44:T49" si="8">IF(AND(Q44="Nicht Gekauft", R44="Benötigt"), P44, 0)</f>
-        <v>8.8000000000000007</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q44" s="41"/>
+      <c r="R44" s="25"/>
       <c r="U44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
       <c r="B45" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>34</v>
+        <v>221</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>45</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>39</v>
+        <v>222</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
+        <v>223</v>
+      </c>
+      <c r="F45" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="G45" s="28">
+        <v>5</v>
+      </c>
       <c r="H45" s="28"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43" t="s">
+      <c r="I45" s="42"/>
+      <c r="J45" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K45" s="43"/>
+      <c r="K45" s="42"/>
       <c r="L45" s="31" t="s">
-        <v>41</v>
+        <v>220</v>
       </c>
       <c r="M45" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N45" s="32">
-        <v>0.56999999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="O45" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P45" s="32">
-        <f t="shared" si="0"/>
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="Q45" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="R45" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="S45" s="6"/>
-      <c r="T45">
-        <f t="shared" si="8"/>
-        <v>2.2799999999999998</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>0.6</v>
+      </c>
+      <c r="Q45" s="33"/>
+      <c r="R45" s="34"/>
       <c r="U45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="35"/>
       <c r="B46" s="35" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C46" s="35" t="s">
         <v>34</v>
       </c>
       <c r="D46" s="35" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E46" s="35" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F46" s="35"/>
       <c r="G46" s="35"/>
@@ -4338,21 +4351,21 @@
       </c>
       <c r="K46" s="38"/>
       <c r="L46" s="39" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="M46" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N46" s="40">
-        <v>0.55000000000000004</v>
+        <v>0.88</v>
       </c>
       <c r="O46" s="41">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="P46" s="40">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="Q46" s="41" t="s">
         <v>21</v>
@@ -4362,65 +4375,63 @@
       </c>
       <c r="S46" s="6"/>
       <c r="T46">
-        <f t="shared" si="8"/>
-        <v>2.2000000000000002</v>
+        <f t="shared" ref="T46:T51" si="8">IF(AND(Q46="Nicht Gekauft", R46="Benötigt"), P46, 0)</f>
+        <v>8.8000000000000007</v>
       </c>
       <c r="U46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
-        <v>70</v>
-      </c>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
       <c r="B47" s="28" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F47" s="28"/>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42" t="s">
+      <c r="I47" s="43"/>
+      <c r="J47" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="K47" s="42"/>
+      <c r="K47" s="43"/>
       <c r="L47" s="31" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="M47" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N47" s="32">
-        <v>1.0900000000000001</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="O47" s="33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P47" s="32">
         <f t="shared" si="0"/>
-        <v>2.1800000000000002</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="Q47" s="33" t="s">
         <v>21</v>
       </c>
       <c r="R47" s="34" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="S47" s="6"/>
       <c r="T47">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="U47">
         <f t="shared" si="2"/>
@@ -4428,58 +4439,54 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="35" t="s">
-        <v>76</v>
-      </c>
+      <c r="A48" s="35"/>
       <c r="B48" s="35" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="D48" s="35" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="E48" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="F48" s="35">
-        <v>4.0000000000000002E-4</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F48" s="35"/>
       <c r="G48" s="35"/>
       <c r="H48" s="35"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="36" t="s">
+      <c r="I48" s="38"/>
+      <c r="J48" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="K48" s="36"/>
+      <c r="K48" s="38"/>
       <c r="L48" s="39" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="M48" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N48" s="40">
-        <v>4.49</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O48" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P48" s="40">
         <f t="shared" si="0"/>
-        <v>8.98</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q48" s="41" t="s">
         <v>21</v>
       </c>
       <c r="R48" s="25" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="S48" s="6"/>
       <c r="T48">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="U48">
         <f t="shared" si="2"/>
@@ -4488,55 +4495,55 @@
     </row>
     <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C49" s="28" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="42"/>
       <c r="J49" s="42" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K49" s="42"/>
       <c r="L49" s="31" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="M49" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>Mouser</v>
+        <v>DigiKey</v>
       </c>
       <c r="N49" s="32">
-        <v>2.81</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="O49" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P49" s="32">
         <f t="shared" si="0"/>
-        <v>11.24</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="Q49" s="33" t="s">
         <v>21</v>
       </c>
       <c r="R49" s="34" t="s">
-        <v>109</v>
+        <v>22</v>
       </c>
       <c r="S49" s="6"/>
       <c r="T49">
         <f t="shared" si="8"/>
-        <v>11.24</v>
+        <v>0</v>
       </c>
       <c r="U49">
         <f t="shared" si="2"/>
@@ -4554,39 +4561,49 @@
         <v>72</v>
       </c>
       <c r="D50" s="35" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="F50" s="35"/>
+        <v>79</v>
+      </c>
+      <c r="F50" s="35">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="G50" s="35"/>
       <c r="H50" s="35"/>
       <c r="I50" s="36"/>
       <c r="J50" s="36" t="s">
-        <v>119</v>
+        <v>36</v>
       </c>
       <c r="K50" s="36"/>
       <c r="L50" s="39" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="M50" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>3D-Jake</v>
+        <v>DigiKey</v>
       </c>
       <c r="N50" s="40">
-        <v>5.99</v>
+        <v>4.49</v>
       </c>
       <c r="O50" s="41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P50" s="40">
-        <f>N50*O50</f>
-        <v>23.96</v>
-      </c>
-      <c r="Q50" s="41"/>
-      <c r="R50" s="25"/>
+        <f t="shared" si="0"/>
+        <v>8.98</v>
+      </c>
+      <c r="Q50" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="R50" s="25" t="s">
+        <v>22</v>
+      </c>
       <c r="S50" s="6"/>
+      <c r="T50">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="U50">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4594,91 +4611,101 @@
     </row>
     <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B51" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="42" t="s">
+      <c r="C51" s="28" t="s">
         <v>72</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="E51" s="28"/>
+        <v>82</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>83</v>
+      </c>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="42"/>
       <c r="J51" s="42" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="K51" s="42"/>
       <c r="L51" s="31" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="M51" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>3D-Jake</v>
+        <v>Mouser</v>
       </c>
       <c r="N51" s="32">
-        <v>2.99</v>
+        <v>2.81</v>
       </c>
       <c r="O51" s="33">
         <v>4</v>
       </c>
       <c r="P51" s="32">
-        <f>N51*O51</f>
-        <v>11.96</v>
-      </c>
-      <c r="Q51" s="33"/>
-      <c r="R51" s="34"/>
+        <f t="shared" si="0"/>
+        <v>11.24</v>
+      </c>
+      <c r="Q51" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="R51" s="34" t="s">
+        <v>109</v>
+      </c>
       <c r="S51" s="6"/>
+      <c r="T51">
+        <f t="shared" si="8"/>
+        <v>11.24</v>
+      </c>
       <c r="U51">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="E52" s="37" t="s">
-        <v>139</v>
+        <v>131</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>132</v>
       </c>
       <c r="F52" s="35"/>
       <c r="G52" s="35"/>
       <c r="H52" s="35"/>
       <c r="I52" s="36"/>
       <c r="J52" s="36" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="K52" s="36"/>
       <c r="L52" s="39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M52" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>DigiKey</v>
+        <v>3D-Jake</v>
       </c>
       <c r="N52" s="40">
-        <v>0.1</v>
+        <v>5.99</v>
       </c>
       <c r="O52" s="41">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="P52" s="40">
         <f>N52*O52</f>
-        <v>1</v>
+        <v>23.96</v>
       </c>
       <c r="Q52" s="41"/>
       <c r="R52" s="25"/>
@@ -4693,41 +4720,39 @@
         <v>70</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
       <c r="C53" s="42" t="s">
         <v>72</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>140</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E53" s="28"/>
       <c r="F53" s="28"/>
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
       <c r="I53" s="42"/>
       <c r="J53" s="42" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="K53" s="42"/>
       <c r="L53" s="31" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="M53" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>DigiKey</v>
+        <v>3D-Jake</v>
       </c>
       <c r="N53" s="32">
-        <v>5.54</v>
+        <v>2.99</v>
       </c>
       <c r="O53" s="33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P53" s="32">
         <f>N53*O53</f>
-        <v>5.54</v>
+        <v>11.96</v>
       </c>
       <c r="Q53" s="33"/>
       <c r="R53" s="34"/>
@@ -4739,19 +4764,19 @@
     </row>
     <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
-        <v>236</v>
+        <v>70</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>237</v>
+        <v>135</v>
       </c>
       <c r="C54" s="36" t="s">
         <v>72</v>
       </c>
       <c r="D54" s="35" t="s">
-        <v>239</v>
-      </c>
-      <c r="E54" s="35" t="s">
-        <v>240</v>
+        <v>134</v>
+      </c>
+      <c r="E54" s="37" t="s">
+        <v>139</v>
       </c>
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
@@ -4762,21 +4787,21 @@
       </c>
       <c r="K54" s="36"/>
       <c r="L54" s="39" t="s">
-        <v>238</v>
+        <v>133</v>
       </c>
       <c r="M54" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N54" s="40">
-        <v>0.19</v>
+        <v>0.1</v>
       </c>
       <c r="O54" s="41">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P54" s="40">
         <f>N54*O54</f>
-        <v>0.19</v>
+        <v>1</v>
       </c>
       <c r="Q54" s="41"/>
       <c r="R54" s="25"/>
@@ -4788,19 +4813,19 @@
     </row>
     <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="C55" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="29" t="s">
-        <v>103</v>
+      <c r="D55" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="F55" s="28"/>
       <c r="G55" s="28"/>
@@ -4811,32 +4836,25 @@
       </c>
       <c r="K55" s="42"/>
       <c r="L55" s="31" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="M55" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N55" s="32">
-        <v>16.100000000000001</v>
+        <v>5.54</v>
       </c>
       <c r="O55" s="33">
         <v>1</v>
       </c>
       <c r="P55" s="32">
-        <f t="shared" si="0"/>
-        <v>16.100000000000001</v>
-      </c>
-      <c r="Q55" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="R55" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="T55">
-        <f>IF(AND(Q55="Nicht Gekauft", R55="Benötigt"), P55, 0)</f>
-        <v>16.100000000000001</v>
-      </c>
+        <f>N55*O55</f>
+        <v>5.54</v>
+      </c>
+      <c r="Q55" s="33"/>
+      <c r="R55" s="34"/>
+      <c r="S55" s="6"/>
       <c r="U55">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4844,55 +4862,56 @@
     </row>
     <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>146</v>
+        <v>235</v>
       </c>
       <c r="B56" s="35" t="s">
-        <v>102</v>
+        <v>236</v>
       </c>
       <c r="C56" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="D56" s="37" t="s">
-        <v>145</v>
+      <c r="D56" s="35" t="s">
+        <v>238</v>
       </c>
       <c r="E56" s="35" t="s">
-        <v>104</v>
+        <v>239</v>
       </c>
       <c r="F56" s="35"/>
       <c r="G56" s="35"/>
       <c r="H56" s="35"/>
       <c r="I56" s="36"/>
       <c r="J56" s="36" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="K56" s="36"/>
       <c r="L56" s="39" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="M56" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>Amazon</v>
+        <v>DigiKey</v>
       </c>
       <c r="N56" s="40">
-        <v>6.99</v>
+        <v>0.19</v>
       </c>
       <c r="O56" s="41">
         <v>1</v>
       </c>
       <c r="P56" s="40">
         <f>N56*O56</f>
-        <v>6.99</v>
+        <v>0.19</v>
       </c>
       <c r="Q56" s="41"/>
       <c r="R56" s="25"/>
+      <c r="S56" s="6"/>
       <c r="U56">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" s="28" t="s">
         <v>102</v>
@@ -4901,38 +4920,46 @@
         <v>72</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="F57" s="28"/>
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
       <c r="I57" s="42"/>
       <c r="J57" s="42" t="s">
-        <v>149</v>
+        <v>36</v>
       </c>
       <c r="K57" s="42"/>
       <c r="L57" s="31" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="M57" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>RobotShop</v>
+        <v>DigiKey</v>
       </c>
       <c r="N57" s="32">
-        <v>9.33</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="O57" s="33">
         <v>1</v>
       </c>
       <c r="P57" s="32">
-        <f>N57*O57</f>
-        <v>9.33</v>
-      </c>
-      <c r="Q57" s="33"/>
-      <c r="R57" s="34"/>
+        <f t="shared" si="0"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q57" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="R57" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="T57">
+        <f>IF(AND(Q57="Nicht Gekauft", R57="Benötigt"), P57, 0)</f>
+        <v>16.100000000000001</v>
+      </c>
       <c r="U57">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4940,7 +4967,7 @@
     </row>
     <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B58" s="35" t="s">
         <v>102</v>
@@ -4949,35 +4976,35 @@
         <v>72</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E58" s="35" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="F58" s="35"/>
       <c r="G58" s="35"/>
       <c r="H58" s="35"/>
       <c r="I58" s="36"/>
       <c r="J58" s="36" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="K58" s="36"/>
       <c r="L58" s="39" t="s">
-        <v>154</v>
+        <v>264</v>
       </c>
       <c r="M58" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>DigiKey</v>
+        <v>Amazon</v>
       </c>
       <c r="N58" s="40">
-        <v>3.39</v>
+        <v>6.99</v>
       </c>
       <c r="O58" s="41">
         <v>1</v>
       </c>
       <c r="P58" s="40">
         <f>N58*O58</f>
-        <v>3.39</v>
+        <v>6.99</v>
       </c>
       <c r="Q58" s="41"/>
       <c r="R58" s="25"/>
@@ -4986,57 +5013,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D59" s="28" t="s">
-        <v>60</v>
+        <v>102</v>
+      </c>
+      <c r="C59" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>147</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="F59" s="28"/>
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
       <c r="I59" s="42"/>
       <c r="J59" s="42" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="K59" s="42"/>
       <c r="L59" s="31" t="s">
-        <v>264</v>
+        <v>150</v>
       </c>
       <c r="M59" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>Amazon</v>
+        <v>RobotShop</v>
       </c>
       <c r="N59" s="32">
-        <v>16.13</v>
+        <v>9.33</v>
       </c>
       <c r="O59" s="33">
         <v>1</v>
       </c>
       <c r="P59" s="32">
-        <f t="shared" si="0"/>
-        <v>16.13</v>
-      </c>
-      <c r="Q59" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="R59" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="T59">
-        <f>IF(AND(Q59="Nicht Gekauft", R59="Benötigt"), P59, 0)</f>
-        <v>16.13</v>
-      </c>
+        <f>N59*O59</f>
+        <v>9.33</v>
+      </c>
+      <c r="Q59" s="33"/>
+      <c r="R59" s="34"/>
       <c r="U59">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5044,19 +5063,19 @@
     </row>
     <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
-        <v>62</v>
+        <v>151</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D60" s="35" t="s">
-        <v>64</v>
+        <v>102</v>
+      </c>
+      <c r="C60" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>152</v>
       </c>
       <c r="E60" s="35" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="F60" s="35"/>
       <c r="G60" s="35"/>
@@ -5067,28 +5086,24 @@
       </c>
       <c r="K60" s="36"/>
       <c r="L60" s="39" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="M60" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N60" s="40">
-        <v>2.97</v>
+        <v>3.39</v>
       </c>
       <c r="O60" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P60" s="40">
-        <f t="shared" si="0"/>
-        <v>5.94</v>
-      </c>
-      <c r="Q60" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="R60" s="25" t="s">
-        <v>22</v>
-      </c>
+        <f>N60*O60</f>
+        <v>3.39</v>
+      </c>
+      <c r="Q60" s="41"/>
+      <c r="R60" s="25"/>
       <c r="U60">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5096,26 +5111,26 @@
     </row>
     <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C61" s="28" t="s">
         <v>57</v>
       </c>
       <c r="D61" s="28" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F61" s="28"/>
       <c r="G61" s="28"/>
       <c r="H61" s="28"/>
       <c r="I61" s="42"/>
       <c r="J61" s="42" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="K61" s="42"/>
       <c r="L61" s="31" t="s">
@@ -5123,23 +5138,27 @@
       </c>
       <c r="M61" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>DigiKey</v>
+        <v>Amazon</v>
       </c>
       <c r="N61" s="32">
-        <v>5.92</v>
+        <v>16.13</v>
       </c>
       <c r="O61" s="33">
         <v>1</v>
       </c>
       <c r="P61" s="32">
         <f t="shared" si="0"/>
-        <v>5.92</v>
+        <v>16.13</v>
       </c>
       <c r="Q61" s="33" t="s">
         <v>21</v>
       </c>
       <c r="R61" s="34" t="s">
-        <v>22</v>
+        <v>109</v>
+      </c>
+      <c r="T61">
+        <f>IF(AND(Q61="Nicht Gekauft", R61="Benötigt"), P61, 0)</f>
+        <v>16.13</v>
       </c>
       <c r="U61">
         <f t="shared" si="2"/>
@@ -5157,7 +5176,7 @@
         <v>57</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E62" s="35" t="s">
         <v>65</v>
@@ -5171,21 +5190,21 @@
       </c>
       <c r="K62" s="36"/>
       <c r="L62" s="39" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M62" s="31" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N62" s="40">
-        <v>2.64</v>
+        <v>2.97</v>
       </c>
       <c r="O62" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P62" s="40">
         <f t="shared" si="0"/>
-        <v>2.64</v>
+        <v>5.94</v>
       </c>
       <c r="Q62" s="41" t="s">
         <v>21</v>
@@ -5193,239 +5212,354 @@
       <c r="R62" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="T62">
-        <f>IF(AND(Q62="Nicht Gekauft", R62="Benötigt"), P62, 0)</f>
-        <v>0</v>
-      </c>
       <c r="U62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="16"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="16"/>
-      <c r="Q63" s="17"/>
-    </row>
-    <row r="65" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F65" s="5" t="s">
+    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="42"/>
+      <c r="J63" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K63" s="42"/>
+      <c r="L63" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="M63" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>DigiKey</v>
+      </c>
+      <c r="N63" s="32">
+        <v>5.92</v>
+      </c>
+      <c r="O63" s="33">
+        <v>1</v>
+      </c>
+      <c r="P63" s="32">
+        <f t="shared" si="0"/>
+        <v>5.92</v>
+      </c>
+      <c r="Q63" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="R63" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="U63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F64" s="35"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="36"/>
+      <c r="J64" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="K64" s="36"/>
+      <c r="L64" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="M64" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>DigiKey</v>
+      </c>
+      <c r="N64" s="40">
+        <v>2.64</v>
+      </c>
+      <c r="O64" s="41">
+        <v>1</v>
+      </c>
+      <c r="P64" s="40">
+        <f t="shared" si="0"/>
+        <v>2.64</v>
+      </c>
+      <c r="Q64" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="R64" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="T64">
+        <f>IF(AND(Q64="Nicht Gekauft", R64="Benötigt"), P64, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="16"/>
+      <c r="Q65" s="17"/>
+    </row>
+    <row r="67" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F67" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="52" t="s">
+        <v>273</v>
+      </c>
+      <c r="G68" s="52" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F69" s="53">
+        <f>SUMPRODUCT(F2:F64, O2:O64, U2:U64)</f>
+        <v>4.2199999999999989</v>
+      </c>
+      <c r="G69" s="53" cm="1">
+        <f t="array" ref="G69">SUMPRODUCT((G2:G64=12)*(F2:F64)*(O2:O64)*(U2:U64))</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>305</v>
+      </c>
+      <c r="C70" t="s">
+        <v>306</v>
+      </c>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>307</v>
+      </c>
+      <c r="C71" t="s">
+        <v>308</v>
+      </c>
+      <c r="G71" s="52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G72" s="53" cm="1">
+        <f t="array" ref="G72">SUMPRODUCT((G2:G64=5)*(F2:F64)*(O2:O64)*(U2:U64))</f>
+        <v>2.04</v>
+      </c>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F74" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="G74" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="66" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F66" s="52" t="s">
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F75" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="G75" s="47" t="s">
         <v>274</v>
       </c>
-      <c r="G66" s="52" t="s">
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F76" s="48">
+        <f>F69*$F$79</f>
+        <v>6.3299999999999983</v>
+      </c>
+      <c r="G76" s="48">
+        <f>G69*$F$79</f>
+        <v>3.2700000000000005</v>
+      </c>
+      <c r="H76" s="3"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+    </row>
+    <row r="77" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F78" s="50" t="s">
+        <v>280</v>
+      </c>
+      <c r="G78" s="47" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="67" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F67" s="53">
-        <f>SUMPRODUCT(F2:F62, O2:O62, U2:U62)</f>
-        <v>4.1599999999999993</v>
-      </c>
-      <c r="G67" s="53" cm="1">
-        <f t="array" ref="G67">SUMPRODUCT((G2:G62=12)*(F2:F62)*(O2:O62)*(U2:U62))</f>
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G69" s="52" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="70" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G70" s="53" cm="1">
-        <f t="array" ref="G70">SUMPRODUCT((G2:G62=5)*(F2:F62)*(O2:O62)*(U2:U62))</f>
-        <v>1.98</v>
-      </c>
-      <c r="H70" s="3"/>
-    </row>
-    <row r="71" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H71" s="3"/>
-    </row>
-    <row r="72" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F72" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="H72" s="3"/>
-    </row>
-    <row r="73" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F73" s="47" t="s">
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F79" s="51">
+        <v>1.5</v>
+      </c>
+      <c r="G79" s="48">
+        <f>G72*$F$79</f>
+        <v>3.06</v>
+      </c>
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="3"/>
+      <c r="I80" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F81" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="82" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F82" s="54" t="s">
+        <v>273</v>
+      </c>
+      <c r="G82" s="55" t="s">
         <v>274</v>
       </c>
-      <c r="G73" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="H73" s="3"/>
-    </row>
-    <row r="74" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F74" s="48">
-        <f>F67*$F$77</f>
-        <v>6.2399999999999984</v>
-      </c>
-      <c r="G74" s="48">
-        <f>G67*$F$77</f>
-        <v>3.2700000000000005</v>
-      </c>
-      <c r="H74" s="3"/>
-      <c r="L74" s="7"/>
-      <c r="M74" s="7"/>
-    </row>
-    <row r="75" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H75" s="3"/>
-    </row>
-    <row r="76" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F76" s="50" t="s">
-        <v>281</v>
-      </c>
-      <c r="G76" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="H76" s="3"/>
-    </row>
-    <row r="77" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F77" s="51">
-        <v>1.5</v>
-      </c>
-      <c r="G77" s="48">
-        <f>G70*$F$77</f>
-        <v>2.9699999999999998</v>
-      </c>
-      <c r="H77" s="3"/>
-    </row>
-    <row r="78" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H78" s="3"/>
-      <c r="I78" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="79" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F79" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="80" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F80" s="54" t="s">
-        <v>274</v>
-      </c>
-      <c r="G80" s="55" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="81" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F81" s="56">
+    </row>
+    <row r="83" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F83" s="56">
         <v>5.5888</v>
       </c>
-      <c r="G81" s="57">
+      <c r="G83" s="57">
         <v>3.04</v>
-      </c>
-    </row>
-    <row r="82" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F82" s="49"/>
-      <c r="G82" s="49"/>
-    </row>
-    <row r="83" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F83" s="49"/>
-      <c r="G83" s="54" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="84" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F84" s="49"/>
-      <c r="G84" s="56">
+      <c r="G84" s="49"/>
+    </row>
+    <row r="85" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F85" s="49"/>
+      <c r="G85" s="54" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="86" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F86" s="49"/>
+      <c r="G86" s="56">
         <v>2.548</v>
-      </c>
-    </row>
-    <row r="86" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F86" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="87" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F87" t="s">
-        <v>291</v>
-      </c>
-      <c r="G87">
-        <v>8</v>
       </c>
     </row>
     <row r="88" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
-        <v>292</v>
-      </c>
-      <c r="G88">
-        <v>5</v>
+        <v>289</v>
       </c>
     </row>
     <row r="89" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G89">
-        <v>0.05</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>291</v>
+      </c>
+      <c r="G90">
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F91" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="92" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F92" t="s">
-        <v>294</v>
-      </c>
-      <c r="G92">
-        <f>G87-G74</f>
-        <v>4.7299999999999995</v>
+        <v>292</v>
+      </c>
+      <c r="G91">
+        <v>0.05</v>
       </c>
     </row>
     <row r="93" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
-        <v>295</v>
-      </c>
-      <c r="G93">
-        <f>G88+G89-G77</f>
-        <v>2.08</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="94" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>293</v>
+      </c>
+      <c r="G94">
+        <f>G89-G76</f>
+        <v>4.7299999999999995</v>
+      </c>
+    </row>
+    <row r="95" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>294</v>
+      </c>
+      <c r="G95">
+        <f>G90+G91-G79</f>
+        <v>1.9899999999999998</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R62" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
+  <autoFilter ref="A1:R64" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="ACC3"/>
         <filter val="BF4"/>
         <filter val="BP2"/>
         <filter val="F2"/>
-        <filter val="POW2"/>
         <filter val="S1"/>
         <filter val="SP2"/>
         <filter val="TP2"/>
@@ -5433,12 +5567,45 @@
     </filterColumn>
   </autoFilter>
   <customSheetViews>
+    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:R60" xr:uid="{5C2FA3F9-BB88-4AE9-BDB1-2634FA3DE481}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A1:R59" xr:uid="{EB4F4FEB-B098-4AD4-A8CB-E1EF5FA87052}"/>
+    </customSheetView>
+    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A1:R59" xr:uid="{12137C77-B4BF-4599-9E37-142A08AB832F}"/>
+    </customSheetView>
     <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:R62" xr:uid="{02D4D05E-22F6-4468-9979-51C6FBB75016}">
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <autoFilter ref="A1:R62" xr:uid="{D499083E-E6EE-4BCD-A092-38E8A2F94FCA}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -5446,39 +5613,6 @@
             <filter val="BP2"/>
             <filter val="F2"/>
             <filter val="POW2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:R59" xr:uid="{80BB990E-581D-4117-B12D-9E1E3A3EDFF2}"/>
-    </customSheetView>
-    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A1:R59" xr:uid="{6817E049-AE4D-453D-9C70-25EEE41FA076}"/>
-    </customSheetView>
-    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A1:R60" xr:uid="{05898425-2B4B-4922-8946-8D2313CCA35E}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
             <filter val="S1"/>
             <filter val="SP2"/>
             <filter val="TP2"/>
@@ -5506,7 +5640,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q25 Q28:Q68 Q70:Q1048576">
+  <conditionalFormatting sqref="Q1:Q25 Q29:Q70 Q72:Q1048576">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Nicht Gekauft"</formula>
     </cfRule>
@@ -5522,7 +5656,7 @@
       <formula>"Gekauft"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R25 R28:R63">
+  <conditionalFormatting sqref="R2:R25 R29:R65">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Nicht benötigt"</formula>
     </cfRule>
@@ -5531,37 +5665,37 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R25 R28:R63" xr:uid="{DF639F38-DCBF-4FB0-9016-BE70B5447265}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R25 R29:R65" xr:uid="{DF639F38-DCBF-4FB0-9016-BE70B5447265}">
       <formula1>"Benötigt,Nicht benötigt"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q25 Q28:Q63" xr:uid="{BB82D80E-695D-4A38-A148-48463DFE8321}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q25 Q29:Q65" xr:uid="{BB82D80E-695D-4A38-A148-48463DFE8321}">
       <formula1>"Gekauft,Nicht Gekauft"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId5" xr:uid="{134576B2-6870-47F8-80B5-95CA9B97F9E2}"/>
-    <hyperlink ref="L44" r:id="rId6" xr:uid="{F3AD9EFC-A933-40C0-B3D6-105AE81F974F}"/>
-    <hyperlink ref="L45" r:id="rId7" xr:uid="{0B081703-43B3-49C1-ABA0-60C83F319C14}"/>
-    <hyperlink ref="L46" r:id="rId8" xr:uid="{A386B0E7-0270-440F-94E8-1A585C273E01}"/>
-    <hyperlink ref="L28" r:id="rId9" xr:uid="{6E8ED221-C460-4F2D-A839-674D0DD8E486}"/>
-    <hyperlink ref="L60" r:id="rId10" xr:uid="{9A0B0992-EB9B-485C-8743-AB5373B961C2}"/>
-    <hyperlink ref="L62" r:id="rId11" xr:uid="{B67FB571-1B87-4184-A2B3-AF411BD87D35}"/>
-    <hyperlink ref="L48" r:id="rId12" xr:uid="{57963C92-CE56-4D91-B1F1-7FA05F5BC3A8}"/>
-    <hyperlink ref="L47" r:id="rId13" xr:uid="{9D795571-0999-43FF-9A1F-496FF99C86C0}"/>
-    <hyperlink ref="L49" r:id="rId14" xr:uid="{8465788D-FDE3-460C-960F-435D2FB5F396}"/>
+    <hyperlink ref="L46" r:id="rId6" xr:uid="{F3AD9EFC-A933-40C0-B3D6-105AE81F974F}"/>
+    <hyperlink ref="L47" r:id="rId7" xr:uid="{0B081703-43B3-49C1-ABA0-60C83F319C14}"/>
+    <hyperlink ref="L48" r:id="rId8" xr:uid="{A386B0E7-0270-440F-94E8-1A585C273E01}"/>
+    <hyperlink ref="L29" r:id="rId9" xr:uid="{6E8ED221-C460-4F2D-A839-674D0DD8E486}"/>
+    <hyperlink ref="L62" r:id="rId10" xr:uid="{9A0B0992-EB9B-485C-8743-AB5373B961C2}"/>
+    <hyperlink ref="L64" r:id="rId11" xr:uid="{B67FB571-1B87-4184-A2B3-AF411BD87D35}"/>
+    <hyperlink ref="L50" r:id="rId12" xr:uid="{57963C92-CE56-4D91-B1F1-7FA05F5BC3A8}"/>
+    <hyperlink ref="L49" r:id="rId13" xr:uid="{9D795571-0999-43FF-9A1F-496FF99C86C0}"/>
+    <hyperlink ref="L51" r:id="rId14" xr:uid="{8465788D-FDE3-460C-960F-435D2FB5F396}"/>
     <hyperlink ref="L10" r:id="rId15" xr:uid="{A9D6150D-3C06-4D81-AD60-047F4F409296}"/>
     <hyperlink ref="L11" r:id="rId16" xr:uid="{411A7094-1AC1-4084-ABE4-5C0060EC1A2D}"/>
     <hyperlink ref="L12" r:id="rId17" xr:uid="{3DDB6C5A-7DB3-4C65-B604-D02293535F49}"/>
     <hyperlink ref="L7" r:id="rId18" xr:uid="{56E44BCE-942A-4E32-8574-907151789664}"/>
-    <hyperlink ref="L55" r:id="rId19" xr:uid="{D632E27D-8B4B-473B-9951-117DBC2C36E0}"/>
+    <hyperlink ref="L57" r:id="rId19" xr:uid="{D632E27D-8B4B-473B-9951-117DBC2C36E0}"/>
     <hyperlink ref="L3" r:id="rId20" xr:uid="{C49F6822-A4DD-42C2-B3BF-0381D137937C}"/>
     <hyperlink ref="L5" r:id="rId21" xr:uid="{BF0FEABB-4850-4BC5-A11D-D889C6B926FD}"/>
     <hyperlink ref="L8" r:id="rId22" xr:uid="{21389653-C0FE-46E1-B136-04B9A0DE28C5}"/>
-    <hyperlink ref="L50" r:id="rId23" xr:uid="{1242A3DC-9FDC-4C47-9270-1B4A92E75E73}"/>
+    <hyperlink ref="L52" r:id="rId23" xr:uid="{1242A3DC-9FDC-4C47-9270-1B4A92E75E73}"/>
     <hyperlink ref="L26" r:id="rId24" xr:uid="{3ED73B15-E49B-4E21-BF8D-06828BFBADB2}"/>
     <hyperlink ref="L9" r:id="rId25" xr:uid="{E62708AD-A075-4D9D-9BC8-2CBD617B66EE}"/>
     <hyperlink ref="L27" r:id="rId26" xr:uid="{488C7B18-56E0-4061-83E3-FAA678922DF9}"/>
-    <hyperlink ref="L32" r:id="rId27" xr:uid="{02A8F53B-7033-433E-97B4-37D43B10ABDE}"/>
+    <hyperlink ref="L33" r:id="rId27" xr:uid="{02A8F53B-7033-433E-97B4-37D43B10ABDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>

</xml_diff>

<commit_message>
fertgie V1 der Leistungs-Platine
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
+++ b/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAA40FB-4947-499C-9F07-3B0A3DAD9FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925D9FAF-93FD-4548-B576-1E185057F4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,10 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
+    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
     <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="353">
   <si>
     <t>Alternative</t>
   </si>
@@ -1085,6 +1085,54 @@
   </si>
   <si>
     <t>https://www.digikey.at/en/products/detail/vishay-dale/IHLP2525CZER3R3M11/5419141</t>
+  </si>
+  <si>
+    <t>Neuer stecker</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>samtec-config</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>https://suddendocs.samtec.com/catalog_english/hle.pdf</t>
+  </si>
+  <si>
+    <t>HLE-107-02-L-DV</t>
+  </si>
+  <si>
+    <t>https://www.samtec.com/products/hle-107-02-l-dv</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/samtec-inc/HLE-107-02-L-DV/6693078</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>allgemeine ressources</t>
+  </si>
+  <si>
+    <t>https://www.samtec.com/flex-stacking/standard/100-pitch-terminals/</t>
+  </si>
+  <si>
+    <t>https://suddendocs.samtec.com/catalog_english/a-tsm.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSM-107-04-L-DV </t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/samtec-inc/TSM-107-04-L-DV/7638934</t>
+  </si>
+  <si>
+    <t>https://www.samtec.com/products/tsm-107-04-l-dv</t>
   </si>
 </sst>
 </file>
@@ -2071,11 +2119,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AD95"/>
+  <dimension ref="A1:AD102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5721,12 +5769,35 @@
         <v>0.05</v>
       </c>
     </row>
+    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>337</v>
+      </c>
+      <c r="B92" t="s">
+        <v>347</v>
+      </c>
+      <c r="C92" t="s">
+        <v>348</v>
+      </c>
+    </row>
     <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>338</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>342</v>
+      </c>
       <c r="F93" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>339</v>
+      </c>
+      <c r="C94" t="s">
+        <v>343</v>
+      </c>
       <c r="F94" t="s">
         <v>293</v>
       </c>
@@ -5736,12 +5807,59 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>340</v>
+      </c>
+      <c r="C95" t="s">
+        <v>341</v>
+      </c>
       <c r="F95" t="s">
         <v>294</v>
       </c>
       <c r="G95">
         <f>G90+G91-G79</f>
         <v>1.9899999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>344</v>
+      </c>
+      <c r="C96" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>346</v>
+      </c>
+      <c r="B99" s="6"/>
+    </row>
+    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>339</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>340</v>
+      </c>
+      <c r="C101" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>344</v>
+      </c>
+      <c r="C102" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -5759,18 +5877,19 @@
     </filterColumn>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
+    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
+      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:R60" xr:uid="{295BE6A1-DF71-41DB-94C7-7837EDCDE11B}">
+      <autoFilter ref="A1:R62" xr:uid="{EEE402BD-B8CC-49C7-A446-2FE651B6D7AC}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
             <filter val="BF4"/>
             <filter val="BP2"/>
             <filter val="F2"/>
+            <filter val="POW2"/>
             <filter val="S1"/>
             <filter val="SP2"/>
             <filter val="TP2"/>
@@ -5778,33 +5897,32 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
+    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A1:R59" xr:uid="{79D92D3E-286D-4993-A74E-06CBA6A73131}"/>
+    </customSheetView>
     <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:R59" xr:uid="{9A3F37CD-16ED-4594-BA05-4EDD4C42FF90}"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A1:R59" xr:uid="{4814F0E0-479A-4F73-9BA7-7AA1FD9D690E}"/>
     </customSheetView>
-    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
+    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A1:R59" xr:uid="{EDDF351F-117D-4CBE-9584-2D660F584372}"/>
-    </customSheetView>
-    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A1:R62" xr:uid="{D2F7AB5A-BFBE-4552-87D4-1589C9F803D8}">
+      <autoFilter ref="A1:R60" xr:uid="{8A29F857-18B3-4055-8510-7E8A92279CCD}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
             <filter val="BF4"/>
             <filter val="BP2"/>
             <filter val="F2"/>
-            <filter val="POW2"/>
             <filter val="S1"/>
             <filter val="SP2"/>
             <filter val="TP2"/>
@@ -5891,8 +6009,11 @@
     <hyperlink ref="C73" r:id="rId28" xr:uid="{F989E443-6F04-45A5-A5B6-83699464B796}"/>
     <hyperlink ref="C74" r:id="rId29" xr:uid="{EA26BA1A-7CE5-4F25-9686-9C9961368AD7}"/>
     <hyperlink ref="C80" r:id="rId30" xr:uid="{627D7733-F0E4-49C3-A927-788CACD174D1}"/>
+    <hyperlink ref="B93" r:id="rId31" display="https://www.samtec.com/products/hle-107-02-l-dv" xr:uid="{05E67635-DC20-4D0B-937A-E1A05B41BF9B}"/>
+    <hyperlink ref="B100" r:id="rId32" display="https://www.samtec.com/products/tsm-107-04-l-dv" xr:uid="{1C96A744-ED9F-48B3-AD1D-5704F3392B1B}"/>
+    <hyperlink ref="C100" r:id="rId33" xr:uid="{9FC22445-D9EC-4755-88E1-E765234394E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
noch mehr bauteile ausgetauscht
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
+++ b/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\GitHub\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054031BB-82EF-44E1-BAE9-2D109C6ABA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5783017-188A-4CC9-BB6D-3E5AEC5B66AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,12 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
+    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Schaltplan_V5" guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
     <customWorkbookView name="Anforderungen_Auswahl" guid="{36C50999-9392-45D3-927D-2C21A30118D3}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_V5" guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="406">
   <si>
     <t>Alternative</t>
   </si>
@@ -1268,9 +1268,6 @@
   </si>
   <si>
     <t>eine moeglichst kompakte bauform haben</t>
-  </si>
-  <si>
-    <t>auf chatgpt chat zurueckgreifen und erklaeren</t>
   </si>
   <si>
     <t>ist aber ueblich in vielen arduino anwendungen</t>
@@ -2294,8 +2291,8 @@
   <dimension ref="A1:AK112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE40" sqref="AE40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5222,9 +5219,6 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AF55" t="s">
-        <v>396</v>
-      </c>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56" s="50"/>
@@ -5275,11 +5269,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="AF56" t="s">
-        <v>390</v>
-      </c>
       <c r="AG56" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.25">
@@ -5332,10 +5323,10 @@
         <v>1</v>
       </c>
       <c r="AF57" t="s">
+        <v>397</v>
+      </c>
+      <c r="AG57" t="s">
         <v>398</v>
-      </c>
-      <c r="AG57" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.25">
@@ -5393,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="AF58" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.25">
@@ -5557,7 +5548,7 @@
       <c r="R61" s="25"/>
       <c r="S61" s="6"/>
       <c r="AF61" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
@@ -5607,7 +5598,7 @@
       <c r="R62" s="25"/>
       <c r="S62" s="6"/>
       <c r="AF62" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.25">
@@ -5726,10 +5717,10 @@
         <v>0</v>
       </c>
       <c r="AF64" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AG64" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.25">
@@ -6034,7 +6025,7 @@
         <v>0</v>
       </c>
       <c r="AF70" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.25">
@@ -6189,7 +6180,7 @@
         <v>0</v>
       </c>
       <c r="AF73" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.25">
@@ -6715,12 +6706,65 @@
     </filterColumn>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{36C50999-9392-45D3-927D-2C21A30118D3}" filter="1" showAutoFilter="1" hiddenColumns="1">
+    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
+      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:R78" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
+      <autoFilter ref="A1:R62" xr:uid="{22EDE2E3-EB50-4243-A545-1DA468F7D7EC}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="POW2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A1:R59" xr:uid="{DC384772-D41A-4AFA-B796-4B9FC8B40975}"/>
+    </customSheetView>
+    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A1:R59" xr:uid="{D75C0060-9AC9-49C2-B86D-0B3FD3CD1453}"/>
+    </customSheetView>
+    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <autoFilter ref="A1:R60" xr:uid="{320774CF-15CF-4906-8E75-067330130449}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+      <autoFilter ref="A1:R78" xr:uid="{392506BF-AE36-465C-AC3C-37C6CDF509DC}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6738,12 +6782,12 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" filter="1" showAutoFilter="1" hiddenColumns="1">
+    <customSheetView guid="{36C50999-9392-45D3-927D-2C21A30118D3}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
+      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:R78" xr:uid="{69666EDC-EA15-4DCB-9AAF-D8F292B9F5C3}">
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+      <autoFilter ref="A1:R78" xr:uid="{4B887387-0E7C-4084-8500-5925343836C9}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6756,59 +6800,6 @@
             <filter val="SP2"/>
             <filter val="ST4"/>
             <filter val="SV2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A1:R60" xr:uid="{3C7ADA09-9C6F-4B79-ADE7-012DC39EF190}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A1:R59" xr:uid="{A29F13EA-2EFA-457E-8488-3154111B2199}"/>
-    </customSheetView>
-    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-      <autoFilter ref="A1:R59" xr:uid="{A1C8DBF2-DBB8-4FDF-9577-BDDF7145CDDC}"/>
-    </customSheetView>
-    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-      <autoFilter ref="A1:R62" xr:uid="{0C0CC385-32C0-44F4-B8AB-5812863E13FD}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="POW2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
             <filter val="TP2"/>
           </filters>
         </filterColumn>

</xml_diff>

<commit_message>
bilder hinzugefuegt, bom bearbeitet
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
+++ b/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\GitHub\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5783017-188A-4CC9-BB6D-3E5AEC5B66AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC420AB-903B-4CB3-B60F-8FE472EC5106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,12 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Anforderungen_Auswahl" guid="{36C50999-9392-45D3-927D-2C21A30118D3}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
+    <customWorkbookView name="Schaltplan_V5" guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
+    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
     <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
-    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_V5" guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
-    <customWorkbookView name="Anforderungen_Auswahl" guid="{36C50999-9392-45D3-927D-2C21A30118D3}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2292,7 +2292,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE40" sqref="AE40"/>
+      <selection pane="bottomLeft" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6706,65 +6706,12 @@
     </filterColumn>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
+    <customSheetView guid="{36C50999-9392-45D3-927D-2C21A30118D3}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
+      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:R62" xr:uid="{22EDE2E3-EB50-4243-A545-1DA468F7D7EC}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="POW2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:R59" xr:uid="{DC384772-D41A-4AFA-B796-4B9FC8B40975}"/>
-    </customSheetView>
-    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A1:R59" xr:uid="{D75C0060-9AC9-49C2-B86D-0B3FD3CD1453}"/>
-    </customSheetView>
-    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A1:R60" xr:uid="{320774CF-15CF-4906-8E75-067330130449}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-      <autoFilter ref="A1:R78" xr:uid="{392506BF-AE36-465C-AC3C-37C6CDF509DC}">
+      <autoFilter ref="A1:R78" xr:uid="{B4F3BF44-7F35-4143-9930-25E8186FF7E9}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6782,12 +6729,12 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{36C50999-9392-45D3-927D-2C21A30118D3}" filter="1" showAutoFilter="1" hiddenColumns="1">
+    <customSheetView guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
+      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-      <autoFilter ref="A1:R78" xr:uid="{4B887387-0E7C-4084-8500-5925343836C9}">
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A1:R78" xr:uid="{FBEFBE2B-D72E-4F13-947F-7414729BFF82}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6800,6 +6747,59 @@
             <filter val="SP2"/>
             <filter val="ST4"/>
             <filter val="SV2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A1:R60" xr:uid="{EA93ABE8-2E41-4C2A-8766-8D8CA804B251}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <autoFilter ref="A1:R59" xr:uid="{41BA9B40-8A1F-4113-8953-025FFA734C02}"/>
+    </customSheetView>
+    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+      <autoFilter ref="A1:R59" xr:uid="{D96542F2-6C6A-44BF-82CF-19E96D686E62}"/>
+    </customSheetView>
+    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+      <autoFilter ref="A1:R62" xr:uid="{D5AD703C-60F1-4B87-AFA2-FE08B386F63B}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="POW2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
             <filter val="TP2"/>
           </filters>
         </filterColumn>

</xml_diff>

<commit_message>
bild hinzugefuegt, step-daten hinzugefuegt, abstandhalter in bom hinzugefuegt
Todos: abstandhalter und neue male-stecker bei leistungsplatine muss im 3d modell geupdated werden, abstandhalter ins 3d modell dazu, 3d modell in inventor zusammenstaellen und als bild auf die platine raufgeben.
pinouts auf der platine machen
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
+++ b/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
@@ -5,38 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\GitHub\fiberprinter-electronics\2nd_mainboard_bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC420AB-903B-4CB3-B60F-8FE472EC5106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3044CC-9660-4855-9570-7ABB49C6B4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2ndMainBoard" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$80</definedName>
     <definedName name="Z_14407C96_79A3_4D80_86DC_7BE14F8182CE_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$I:$I,'2ndMainBoard'!$M:$M,'2ndMainBoard'!$P:$R,'2ndMainBoard'!$T:$AD</definedName>
-    <definedName name="Z_14407C96_79A3_4D80_86DC_7BE14F8182CE_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$78</definedName>
+    <definedName name="Z_14407C96_79A3_4D80_86DC_7BE14F8182CE_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$80</definedName>
     <definedName name="Z_36C50999_9392_45D3_927D_2C21A30118D3_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$F:$L,'2ndMainBoard'!$O:$AD</definedName>
-    <definedName name="Z_36C50999_9392_45D3_927D_2C21A30118D3_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$78</definedName>
+    <definedName name="Z_36C50999_9392_45D3_927D_2C21A30118D3_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$80</definedName>
     <definedName name="Z_86D49B71_F0A7_4EDF_9F83_437E8F1DE26F_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$H:$L,'2ndMainBoard'!$Q:$R,'2ndMainBoard'!$T:$U</definedName>
-    <definedName name="Z_86D49B71_F0A7_4EDF_9F83_437E8F1DE26F_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$78</definedName>
+    <definedName name="Z_86D49B71_F0A7_4EDF_9F83_437E8F1DE26F_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$80</definedName>
     <definedName name="Z_AD0CFDC5_A886_4774_8323_B873BC9D36B7_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$F:$L,'2ndMainBoard'!$Q:$R,'2ndMainBoard'!$T:$V</definedName>
-    <definedName name="Z_AD0CFDC5_A886_4774_8323_B873BC9D36B7_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$78</definedName>
+    <definedName name="Z_AD0CFDC5_A886_4774_8323_B873BC9D36B7_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$80</definedName>
     <definedName name="Z_B27C99E1_F194_4CDD_BEEF_0E7944A43981_.wvu.Cols" localSheetId="0" hidden="1">'2ndMainBoard'!$F:$L,'2ndMainBoard'!$Q:$R,'2ndMainBoard'!$T:$V</definedName>
-    <definedName name="Z_B27C99E1_F194_4CDD_BEEF_0E7944A43981_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$78</definedName>
-    <definedName name="Z_E3E09E1D_E21B_434F_8777_BA2F5DFE998D_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$78</definedName>
+    <definedName name="Z_B27C99E1_F194_4CDD_BEEF_0E7944A43981_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$80</definedName>
+    <definedName name="Z_E3E09E1D_E21B_434F_8777_BA2F5DFE998D_.wvu.FilterData" localSheetId="0" hidden="1">'2ndMainBoard'!$A$1:$R$80</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
+    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Schaltplan_V5" guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
     <customWorkbookView name="Anforderungen_Auswahl" guid="{36C50999-9392-45D3-927D-2C21A30118D3}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_V5" guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_Strombudget_V3" guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Default_V2" guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan_V4" guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="417">
   <si>
     <t>Alternative</t>
   </si>
@@ -1072,9 +1072,6 @@
     <t>SV2</t>
   </si>
   <si>
-    <t>8 Reihenpaare, ohne Location Peg</t>
-  </si>
-  <si>
     <t>config: https://www.samtec.com/products/tsm-107-04-l-dv pdf: https://suddendocs.samtec.com/catalog_english/a-tsm.pdf allgemein: https://www.samtec.com/flex-stacking/standard/100-pitch-terminals/</t>
   </si>
   <si>
@@ -1298,6 +1295,42 @@
   </si>
   <si>
     <t>sollte mit klipper kompatibel sein und eine moeglichst kleine bauform haben und unkompliziert sein, sowie ueber i2c auslesbar sein.</t>
+  </si>
+  <si>
+    <t>Steckverbinder Male, Hoch</t>
+  </si>
+  <si>
+    <t>HW-07-08-L-D-250-SM</t>
+  </si>
+  <si>
+    <t>7 Reihenpaare, ohne Location Peg, 11mm hoch</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Samtec/HW-07-08-L-D-250-SM?qs=3%252BjIH0OdpA8a62QJxWcTNw%3D%3D</t>
+  </si>
+  <si>
+    <t>ist auf DigiKey nur in 32er Pakten erähtlich; config: https://www.samtec.com/products/hw-07-08-l-d-250-sm</t>
+  </si>
+  <si>
+    <t>soll in der hoehe gestapelt so niedrig wie moeglich sein</t>
+  </si>
+  <si>
+    <t>soll zur female-buchse passen und eine gesamthoehe von ca 7mm ergeben</t>
+  </si>
+  <si>
+    <t>das gleiche</t>
+  </si>
+  <si>
+    <t>soll zur female-buchse passen und eine gesamthoehe von ca 11-12mm haben, damit sich die leistungsbuchse von der hoehe her ausgeht</t>
+  </si>
+  <si>
+    <t>ist fuer die verbindung zwischen fan und leistungsplatine gedacht, sollte also ca 7mm hoch sein</t>
+  </si>
+  <si>
+    <t>11mm Abstandhalter</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/w%C3%BCrth-elektronik/971110154/9488627</t>
   </si>
 </sst>
 </file>
@@ -1899,9 +1932,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20 % - Akzent1" xfId="2" builtinId="30"/>
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -2288,14 +2321,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AK112"/>
+  <dimension ref="A1:AK114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M34" sqref="M34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF85" sqref="AF85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
@@ -2390,22 +2423,22 @@
       </c>
       <c r="Y1" s="58"/>
       <c r="Z1" s="11">
-        <f>SUMIFS(P10:P78,Q10:Q78, "Nicht Gekauft",R10:R78,"Benötigt")</f>
-        <v>64.3</v>
+        <f>SUMIFS(P10:P80,Q10:Q80, "Nicht Gekauft",R10:R80,"Benötigt")</f>
+        <v>59.019999999999996</v>
       </c>
       <c r="AB1" s="55" t="s">
         <v>106</v>
       </c>
       <c r="AC1" s="56"/>
       <c r="AD1" s="10">
-        <f>SUM(P2:P78)</f>
-        <v>457.60000000000008</v>
+        <f>SUM(P2:P80)</f>
+        <v>457.49000000000007</v>
       </c>
       <c r="AF1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AH1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -2444,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="29">
-        <f t="shared" ref="P2:P78" si="0">N2*O2</f>
+        <f t="shared" ref="P2:P80" si="0">N2*O2</f>
         <v>9.91</v>
       </c>
       <c r="Q2" s="30" t="s">
@@ -2462,10 +2495,10 @@
         <v>0</v>
       </c>
       <c r="AF2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>114</v>
       </c>
@@ -2497,7 +2530,7 @@
         <v>27</v>
       </c>
       <c r="M3" s="50" t="str">
-        <f t="shared" ref="M3:M66" si="1">HYPERLINK(L3,J3)</f>
+        <f t="shared" ref="M3:M68" si="1">HYPERLINK(L3,J3)</f>
         <v>AZ-Delivery</v>
       </c>
       <c r="N3" s="52">
@@ -2517,14 +2550,14 @@
         <v>108</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U78" si="2">SUBTOTAL(103, G3)</f>
+        <f t="shared" ref="U3:U80" si="2">SUBTOTAL(103, G3)</f>
         <v>1</v>
       </c>
       <c r="AF3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>115</v>
       </c>
@@ -2573,7 +2606,7 @@
       <c r="R4" s="31"/>
       <c r="U4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="5"/>
@@ -2640,14 +2673,14 @@
       </c>
       <c r="Y5" s="62"/>
       <c r="Z5" s="12">
-        <f>SUBTOTAL(9,P1:P78)</f>
-        <v>421.13000000000011</v>
+        <f>SUBTOTAL(9,P1:P80)</f>
+        <v>252.74999999999997</v>
       </c>
       <c r="AF5" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
         <v>263</v>
       </c>
@@ -2704,10 +2737,10 @@
       <c r="Y6" s="36"/>
       <c r="Z6" s="37"/>
       <c r="AF6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
         <v>122</v>
       </c>
@@ -2765,15 +2798,15 @@
       </c>
       <c r="U7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X7" s="59" t="s">
         <v>109</v>
       </c>
       <c r="Y7" s="60"/>
       <c r="Z7" s="9">
-        <f>SUBTOTAL(9,T1:T78)</f>
-        <v>89.28</v>
+        <f>SUBTOTAL(9,T1:T80)</f>
+        <v>10.51</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
@@ -2830,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="AF8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
@@ -2887,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>166</v>
       </c>
@@ -2945,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
         <v>166</v>
       </c>
@@ -3003,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
         <v>166</v>
       </c>
@@ -3061,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50" t="s">
         <v>167</v>
       </c>
@@ -3119,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
         <v>168</v>
       </c>
@@ -3169,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50" t="s">
         <v>169</v>
       </c>
@@ -3277,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
@@ -3329,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="AF17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
@@ -3381,15 +3414,15 @@
         <v>0</v>
       </c>
       <c r="AF18" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
+        <v>332</v>
+      </c>
+      <c r="B19" s="50" t="s">
         <v>333</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>334</v>
       </c>
       <c r="C19" s="50" t="s">
         <v>173</v>
@@ -3398,7 +3431,7 @@
         <v>301</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F19" s="50"/>
       <c r="G19" s="50"/>
@@ -3431,12 +3464,12 @@
       <c r="R19" s="25"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C20" s="50" t="s">
         <v>173</v>
@@ -3445,7 +3478,7 @@
         <v>299</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F20" s="50"/>
       <c r="G20" s="50"/>
@@ -3478,12 +3511,12 @@
       <c r="R20" s="25"/>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
+        <v>337</v>
+      </c>
+      <c r="B21" s="50" t="s">
         <v>338</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>339</v>
       </c>
       <c r="C21" s="50" t="s">
         <v>173</v>
@@ -3492,7 +3525,7 @@
         <v>303</v>
       </c>
       <c r="E21" s="50" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
@@ -3523,12 +3556,12 @@
       <c r="R21" s="25"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C22" s="50" t="s">
         <v>173</v>
@@ -3537,7 +3570,7 @@
         <v>5013300200</v>
       </c>
       <c r="E22" s="50" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -3570,12 +3603,12 @@
       <c r="R22" s="25"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C23" s="50" t="s">
         <v>173</v>
@@ -3584,7 +3617,7 @@
         <v>665103131822</v>
       </c>
       <c r="E23" s="50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F23" s="50"/>
       <c r="G23" s="50"/>
@@ -3617,12 +3650,12 @@
       <c r="R23" s="25"/>
       <c r="S23" s="8"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C24" s="50" t="s">
         <v>173</v>
@@ -3631,7 +3664,7 @@
         <v>665003113322</v>
       </c>
       <c r="E24" s="50" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F24" s="50"/>
       <c r="G24" s="50"/>
@@ -3664,12 +3697,12 @@
       <c r="R24" s="25"/>
       <c r="S24" s="8"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="B25" s="50" t="s">
         <v>346</v>
-      </c>
-      <c r="B25" s="50" t="s">
-        <v>347</v>
       </c>
       <c r="C25" s="50" t="s">
         <v>173</v>
@@ -3678,10 +3711,10 @@
         <v>310</v>
       </c>
       <c r="E25" s="50" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F25" s="50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G25" s="50"/>
       <c r="H25" s="50">
@@ -3713,21 +3746,21 @@
       <c r="R25" s="25"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D26" s="50" t="s">
         <v>312</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F26" s="50"/>
       <c r="G26" s="50"/>
@@ -3760,12 +3793,12 @@
       <c r="R26" s="25"/>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="50" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C27" s="50" t="s">
         <v>173</v>
@@ -3774,7 +3807,7 @@
         <v>314</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F27" s="50"/>
       <c r="G27" s="50"/>
@@ -3809,19 +3842,19 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="50" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D28" s="50">
         <v>665002113322</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F28" s="50"/>
       <c r="G28" s="50"/>
@@ -3854,24 +3887,24 @@
       <c r="R28" s="25"/>
       <c r="S28" s="8"/>
       <c r="AF28" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="50" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B29" s="50" t="s">
+        <v>356</v>
+      </c>
+      <c r="C29" s="50" t="s">
         <v>357</v>
-      </c>
-      <c r="C29" s="50" t="s">
-        <v>358</v>
       </c>
       <c r="D29" s="50">
         <v>665102131822</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F29" s="50"/>
       <c r="G29" s="50"/>
@@ -3904,10 +3937,10 @@
       <c r="R29" s="25"/>
       <c r="S29" s="8"/>
       <c r="AF29" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50" t="s">
         <v>179</v>
       </c>
@@ -3915,7 +3948,7 @@
         <v>178</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D30" s="50" t="s">
         <v>177</v>
@@ -3966,7 +3999,7 @@
         <v>178</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D31" s="50" t="s">
         <v>181</v>
@@ -4007,13 +4040,13 @@
         <v>0</v>
       </c>
       <c r="AE31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF31" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50" t="s">
         <v>193</v>
       </c>
@@ -4021,7 +4054,7 @@
         <v>184</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D32" s="50" t="s">
         <v>186</v>
@@ -4072,7 +4105,7 @@
         <v>184</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D33" s="50" t="s">
         <v>189</v>
@@ -4113,16 +4146,16 @@
         <v>0</v>
       </c>
       <c r="AE33" t="s">
+        <v>376</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>374</v>
+      </c>
+      <c r="AG33" t="s">
         <v>377</v>
       </c>
-      <c r="AF33" t="s">
-        <v>375</v>
-      </c>
-      <c r="AG33" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:37" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
         <v>195</v>
       </c>
@@ -4130,7 +4163,7 @@
         <v>184</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D34" s="50" t="s">
         <v>190</v>
@@ -4177,7 +4210,7 @@
         <v>201</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D35" s="50" t="s">
         <v>202</v>
@@ -4217,7 +4250,7 @@
         <v>0</v>
       </c>
       <c r="AF35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4268,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="AE36" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:37" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4362,10 +4395,10 @@
       <c r="Q38" s="28"/>
       <c r="R38" s="28"/>
       <c r="AF38" t="s">
+        <v>380</v>
+      </c>
+      <c r="AG38" t="s">
         <v>381</v>
-      </c>
-      <c r="AG38" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
@@ -4576,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="AF42" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
@@ -4625,7 +4658,7 @@
         <v>0</v>
       </c>
       <c r="AF43" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
@@ -4674,13 +4707,13 @@
         <v>0</v>
       </c>
       <c r="AF44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="50"/>
       <c r="B45" s="50" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C45" s="54" t="s">
         <v>228</v>
@@ -4719,16 +4752,16 @@
       <c r="Q45" s="30"/>
       <c r="R45" s="31"/>
       <c r="AF45" t="s">
+        <v>385</v>
+      </c>
+      <c r="AK45" t="s">
         <v>386</v>
-      </c>
-      <c r="AK45" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="50"/>
       <c r="B46" s="50" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C46" s="54" t="s">
         <v>228</v>
@@ -4767,10 +4800,10 @@
       <c r="Q46" s="30"/>
       <c r="R46" s="31"/>
       <c r="AF46" t="s">
+        <v>385</v>
+      </c>
+      <c r="AK46" t="s">
         <v>386</v>
-      </c>
-      <c r="AK46" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
@@ -4819,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="AF47" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4868,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="AF48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.25">
@@ -4917,7 +4950,7 @@
         <v>0</v>
       </c>
       <c r="AF49" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="50" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
@@ -4964,7 +4997,7 @@
       <c r="Q50" s="34"/>
       <c r="R50" s="25"/>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
         <v>276</v>
       </c>
@@ -5012,7 +5045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="50" t="s">
         <v>276</v>
       </c>
@@ -5108,13 +5141,13 @@
       <c r="Q53" s="30"/>
       <c r="R53" s="31"/>
       <c r="AF53" t="s">
+        <v>390</v>
+      </c>
+      <c r="AG53" t="s">
         <v>391</v>
       </c>
-      <c r="AG53" t="s">
+      <c r="AH53" t="s">
         <v>392</v>
-      </c>
-      <c r="AH53" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.25">
@@ -5161,13 +5194,13 @@
       <c r="Q54" s="34"/>
       <c r="R54" s="25"/>
       <c r="AF54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AG54" t="s">
+        <v>393</v>
+      </c>
+      <c r="AH54" t="s">
         <v>394</v>
-      </c>
-      <c r="AH54" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.25">
@@ -5270,7 +5303,7 @@
         <v>1</v>
       </c>
       <c r="AG56" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.25">
@@ -5323,10 +5356,10 @@
         <v>1</v>
       </c>
       <c r="AF57" t="s">
+        <v>396</v>
+      </c>
+      <c r="AG57" t="s">
         <v>397</v>
-      </c>
-      <c r="AG57" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.25">
@@ -5337,8 +5370,8 @@
       <c r="C58" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="D58" s="50" t="s">
-        <v>31</v>
+      <c r="D58" s="50">
+        <v>971070154</v>
       </c>
       <c r="E58" s="50" t="s">
         <v>34</v>
@@ -5362,11 +5395,11 @@
         <v>0.88</v>
       </c>
       <c r="O58" s="53">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="P58" s="33">
         <f t="shared" si="0"/>
-        <v>8.8000000000000007</v>
+        <v>3.52</v>
       </c>
       <c r="Q58" s="34" t="s">
         <v>21</v>
@@ -5376,32 +5409,33 @@
       </c>
       <c r="S58" s="6"/>
       <c r="T58">
-        <f t="shared" ref="T58:T65" si="7">IF(AND(Q58="Nicht Gekauft", R58="Benötigt"), P58, 0)</f>
-        <v>8.8000000000000007</v>
+        <f t="shared" ref="T58:T67" si="7">IF(AND(Q58="Nicht Gekauft", R58="Benötigt"), P58, 0)</f>
+        <v>3.52</v>
       </c>
       <c r="U58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF58" t="s">
-        <v>399</v>
+        <v>398</v>
+      </c>
+      <c r="AG58" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A59" s="50" t="s">
-        <v>326</v>
-      </c>
+      <c r="A59" s="50"/>
       <c r="B59" s="50" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C59" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="D59" s="50" t="s">
-        <v>38</v>
+      <c r="D59" s="50">
+        <v>971110154</v>
       </c>
       <c r="E59" s="50" t="s">
-        <v>39</v>
+        <v>415</v>
       </c>
       <c r="F59" s="50"/>
       <c r="G59" s="50"/>
@@ -5412,50 +5446,38 @@
       </c>
       <c r="K59" s="54"/>
       <c r="L59" s="50" t="s">
-        <v>40</v>
+        <v>416</v>
       </c>
       <c r="M59" s="50" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N59" s="52">
-        <v>0.56999999999999995</v>
+        <v>0.75</v>
       </c>
       <c r="O59" s="53">
         <v>4</v>
       </c>
-      <c r="P59" s="29">
+      <c r="P59" s="33">
         <f t="shared" si="0"/>
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="Q59" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="R59" s="31" t="s">
-        <v>108</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="Q59" s="34"/>
+      <c r="R59" s="25"/>
       <c r="S59" s="6"/>
-      <c r="T59">
-        <f t="shared" si="7"/>
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="U59">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="50" t="s">
         <v>326</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C60" s="50" t="s">
         <v>325</v>
       </c>
       <c r="D60" s="50" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E60" s="50" t="s">
         <v>39</v>
@@ -5469,53 +5491,53 @@
       </c>
       <c r="K60" s="54"/>
       <c r="L60" s="50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M60" s="50" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N60" s="52">
-        <v>0.55000000000000004</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="O60" s="53">
         <v>4</v>
       </c>
       <c r="P60" s="33">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Q60" s="34" t="s">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="Q60" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="R60" s="25" t="s">
+      <c r="R60" s="31" t="s">
         <v>108</v>
       </c>
       <c r="S60" s="6"/>
       <c r="T60">
         <f t="shared" si="7"/>
-        <v>2.2000000000000002</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="U60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="50" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C61" s="50" t="s">
         <v>325</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>321</v>
+        <v>42</v>
       </c>
       <c r="E61" s="50" t="s">
-        <v>328</v>
+        <v>39</v>
       </c>
       <c r="F61" s="50"/>
       <c r="G61" s="50"/>
@@ -5524,31 +5546,38 @@
       <c r="J61" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="K61" s="50" t="s">
-        <v>327</v>
-      </c>
+      <c r="K61" s="54"/>
       <c r="L61" s="50" t="s">
-        <v>322</v>
+        <v>43</v>
       </c>
       <c r="M61" s="50" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N61" s="52">
-        <v>2.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O61" s="53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P61" s="33">
         <f t="shared" si="0"/>
-        <v>5.2</v>
-      </c>
-      <c r="Q61" s="34"/>
-      <c r="R61" s="25"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q61" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="R61" s="25" t="s">
+        <v>108</v>
+      </c>
       <c r="S61" s="6"/>
-      <c r="AF61" t="s">
-        <v>400</v>
+      <c r="T61">
+        <f t="shared" si="7"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
@@ -5556,16 +5585,16 @@
         <v>329</v>
       </c>
       <c r="B62" s="50" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C62" s="50" t="s">
         <v>325</v>
       </c>
       <c r="D62" s="50" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E62" s="50" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F62" s="50"/>
       <c r="G62" s="50"/>
@@ -5575,47 +5604,50 @@
         <v>35</v>
       </c>
       <c r="K62" s="50" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="L62" s="50" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="M62" s="50" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N62" s="52">
-        <v>1.53</v>
+        <v>2.6</v>
       </c>
       <c r="O62" s="53">
         <v>2</v>
       </c>
       <c r="P62" s="33">
         <f t="shared" si="0"/>
-        <v>3.06</v>
+        <v>5.2</v>
       </c>
       <c r="Q62" s="34"/>
       <c r="R62" s="25"/>
       <c r="S62" s="6"/>
       <c r="AF62" t="s">
-        <v>401</v>
+        <v>399</v>
+      </c>
+      <c r="AG62" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63" s="50" t="s">
-        <v>69</v>
+        <v>329</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="C63" s="50" t="s">
-        <v>71</v>
+        <v>325</v>
       </c>
       <c r="D63" s="50" t="s">
-        <v>72</v>
+        <v>323</v>
       </c>
       <c r="E63" s="50" t="s">
-        <v>73</v>
+        <v>328</v>
       </c>
       <c r="F63" s="50"/>
       <c r="G63" s="50"/>
@@ -5624,163 +5656,147 @@
       <c r="J63" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="K63" s="54"/>
+      <c r="K63" s="50" t="s">
+        <v>330</v>
+      </c>
       <c r="L63" s="50" t="s">
-        <v>74</v>
+        <v>324</v>
       </c>
       <c r="M63" s="50" t="str">
         <f t="shared" si="1"/>
         <v>DigiKey</v>
       </c>
       <c r="N63" s="52">
-        <v>1.0900000000000001</v>
+        <v>1.53</v>
       </c>
       <c r="O63" s="53">
         <v>2</v>
       </c>
-      <c r="P63" s="29">
+      <c r="P63" s="33">
         <f t="shared" si="0"/>
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="Q63" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="R63" s="31" t="s">
-        <v>22</v>
-      </c>
+        <v>3.06</v>
+      </c>
+      <c r="Q63" s="34"/>
+      <c r="R63" s="25"/>
       <c r="S63" s="6"/>
-      <c r="T63">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="U63">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="AF63" t="s">
+        <v>400</v>
+      </c>
+      <c r="AG63" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" s="50" t="s">
-        <v>75</v>
+        <v>329</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>76</v>
+        <v>405</v>
       </c>
       <c r="C64" s="50" t="s">
-        <v>71</v>
+        <v>325</v>
       </c>
       <c r="D64" s="50" t="s">
-        <v>77</v>
+        <v>406</v>
       </c>
       <c r="E64" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="F64" s="50">
-        <v>4.0000000000000002E-4</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="F64" s="50"/>
       <c r="G64" s="50"/>
       <c r="H64" s="50"/>
       <c r="I64" s="54"/>
       <c r="J64" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="K64" s="54"/>
+        <v>45</v>
+      </c>
+      <c r="K64" s="50" t="s">
+        <v>409</v>
+      </c>
       <c r="L64" s="50" t="s">
-        <v>79</v>
+        <v>408</v>
       </c>
       <c r="M64" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>DigiKey</v>
+        <v>Mouser</v>
       </c>
       <c r="N64" s="52">
-        <v>4.49</v>
+        <v>2.17</v>
       </c>
       <c r="O64" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P64" s="33">
         <f t="shared" si="0"/>
-        <v>8.98</v>
-      </c>
-      <c r="Q64" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="R64" s="25" t="s">
-        <v>22</v>
-      </c>
+        <v>2.17</v>
+      </c>
+      <c r="Q64" s="34"/>
+      <c r="R64" s="25"/>
       <c r="S64" s="6"/>
-      <c r="T64">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="U64">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="AF64" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="AG64" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="65" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="50" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B65" s="50" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C65" s="50" t="s">
         <v>71</v>
       </c>
       <c r="D65" s="50" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E65" s="50" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F65" s="50"/>
       <c r="G65" s="50"/>
       <c r="H65" s="50"/>
       <c r="I65" s="54"/>
       <c r="J65" s="54" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="K65" s="54"/>
       <c r="L65" s="50" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M65" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>Mouser</v>
+        <v>DigiKey</v>
       </c>
       <c r="N65" s="52">
-        <v>2.81</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="O65" s="53">
-        <v>4</v>
-      </c>
-      <c r="P65" s="29">
+        <v>2</v>
+      </c>
+      <c r="P65" s="33">
         <f t="shared" si="0"/>
-        <v>11.24</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="Q65" s="30" t="s">
         <v>21</v>
       </c>
       <c r="R65" s="31" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="S65" s="6"/>
       <c r="T65">
         <f t="shared" si="7"/>
-        <v>11.24</v>
+        <v>0</v>
       </c>
       <c r="U65">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="50" t="s">
         <v>75</v>
       </c>
@@ -5791,135 +5807,161 @@
         <v>71</v>
       </c>
       <c r="D66" s="50" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
       <c r="E66" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="F66" s="50"/>
+        <v>78</v>
+      </c>
+      <c r="F66" s="50">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="G66" s="50"/>
       <c r="H66" s="50"/>
       <c r="I66" s="54"/>
       <c r="J66" s="54" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="K66" s="54"/>
       <c r="L66" s="50" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="M66" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>3D-Jake</v>
+        <v>DigiKey</v>
       </c>
       <c r="N66" s="52">
-        <v>5.99</v>
+        <v>4.49</v>
       </c>
       <c r="O66" s="53">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P66" s="33">
-        <f>N66*O66</f>
-        <v>23.96</v>
+        <f t="shared" si="0"/>
+        <v>8.98</v>
       </c>
       <c r="Q66" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="R66" s="25"/>
+        <v>21</v>
+      </c>
+      <c r="R66" s="25" t="s">
+        <v>22</v>
+      </c>
       <c r="S66" s="6"/>
+      <c r="T66">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="U66">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF66" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG66" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="67" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="50" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B67" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="54" t="s">
+      <c r="C67" s="50" t="s">
         <v>71</v>
       </c>
       <c r="D67" s="50" t="s">
-        <v>141</v>
-      </c>
-      <c r="E67" s="50"/>
+        <v>81</v>
+      </c>
+      <c r="E67" s="50" t="s">
+        <v>82</v>
+      </c>
       <c r="F67" s="50"/>
       <c r="G67" s="50"/>
       <c r="H67" s="50"/>
       <c r="I67" s="54"/>
       <c r="J67" s="54" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="K67" s="54"/>
       <c r="L67" s="50" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="M67" s="50" t="str">
-        <f t="shared" ref="M67:M77" si="8">HYPERLINK(L67,J67)</f>
-        <v>3D-Jake</v>
+        <f t="shared" si="1"/>
+        <v>Mouser</v>
       </c>
       <c r="N67" s="52">
-        <v>2.99</v>
+        <v>2.81</v>
       </c>
       <c r="O67" s="53">
         <v>4</v>
       </c>
-      <c r="P67" s="29">
-        <f>N67*O67</f>
-        <v>11.96</v>
-      </c>
-      <c r="Q67" s="30"/>
-      <c r="R67" s="31"/>
+      <c r="P67" s="33">
+        <f t="shared" si="0"/>
+        <v>11.24</v>
+      </c>
+      <c r="Q67" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="R67" s="31" t="s">
+        <v>108</v>
+      </c>
       <c r="S67" s="6"/>
+      <c r="T67">
+        <f t="shared" si="7"/>
+        <v>11.24</v>
+      </c>
       <c r="U67">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" s="50" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" s="50" t="s">
         <v>71</v>
       </c>
       <c r="D68" s="50" t="s">
-        <v>133</v>
-      </c>
-      <c r="E68" s="51" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="E68" s="50" t="s">
+        <v>131</v>
       </c>
       <c r="F68" s="50"/>
       <c r="G68" s="50"/>
       <c r="H68" s="50"/>
       <c r="I68" s="54"/>
       <c r="J68" s="54" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="K68" s="54"/>
       <c r="L68" s="50" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="M68" s="50" t="str">
-        <f>HYPERLINK(L68,J68)</f>
-        <v>DigiKey</v>
+        <f t="shared" si="1"/>
+        <v>3D-Jake</v>
       </c>
       <c r="N68" s="52">
-        <v>0.1</v>
+        <v>5.99</v>
       </c>
       <c r="O68" s="53">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="P68" s="33">
         <f>N68*O68</f>
-        <v>1</v>
-      </c>
-      <c r="Q68" s="34"/>
+        <v>23.96</v>
+      </c>
+      <c r="Q68" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="R68" s="25"/>
       <c r="S68" s="6"/>
       <c r="U68">
@@ -5927,46 +5969,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="50" t="s">
         <v>69</v>
       </c>
       <c r="B69" s="50" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="C69" s="54" t="s">
         <v>71</v>
       </c>
       <c r="D69" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="E69" s="50" t="s">
-        <v>139</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="E69" s="50"/>
       <c r="F69" s="50"/>
       <c r="G69" s="50"/>
       <c r="H69" s="50"/>
       <c r="I69" s="54"/>
       <c r="J69" s="54" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="K69" s="54"/>
       <c r="L69" s="50" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M69" s="50" t="str">
-        <f t="shared" si="8"/>
-        <v>DigiKey</v>
+        <f t="shared" ref="M69:M79" si="8">HYPERLINK(L69,J69)</f>
+        <v>3D-Jake</v>
       </c>
       <c r="N69" s="52">
-        <v>5.54</v>
+        <v>2.99</v>
       </c>
       <c r="O69" s="53">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P69" s="29">
         <f>N69*O69</f>
-        <v>5.54</v>
+        <v>11.96</v>
       </c>
       <c r="Q69" s="30"/>
       <c r="R69" s="31"/>
@@ -5976,21 +6016,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="50" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B70" s="50" t="s">
-        <v>231</v>
+        <v>134</v>
       </c>
       <c r="C70" s="54" t="s">
         <v>71</v>
       </c>
       <c r="D70" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="E70" s="50" t="s">
-        <v>234</v>
+        <v>133</v>
+      </c>
+      <c r="E70" s="51" t="s">
+        <v>138</v>
       </c>
       <c r="F70" s="50"/>
       <c r="G70" s="50"/>
@@ -6001,21 +6041,21 @@
       </c>
       <c r="K70" s="54"/>
       <c r="L70" s="50" t="s">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="M70" s="50" t="str">
-        <f t="shared" si="8"/>
+        <f>HYPERLINK(L70,J70)</f>
         <v>DigiKey</v>
       </c>
       <c r="N70" s="52">
-        <v>0.19</v>
+        <v>0.1</v>
       </c>
       <c r="O70" s="53">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P70" s="33">
         <f>N70*O70</f>
-        <v>0.19</v>
+        <v>1</v>
       </c>
       <c r="Q70" s="34"/>
       <c r="R70" s="25"/>
@@ -6024,25 +6064,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF70" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="50" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="B71" s="50" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="C71" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="D71" s="51" t="s">
-        <v>102</v>
+      <c r="D71" s="50" t="s">
+        <v>135</v>
       </c>
       <c r="E71" s="50" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="F71" s="50"/>
       <c r="G71" s="50"/>
@@ -6053,88 +6090,85 @@
       </c>
       <c r="K71" s="54"/>
       <c r="L71" s="50" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="M71" s="50" t="str">
         <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N71" s="52">
-        <v>16.100000000000001</v>
+        <v>5.54</v>
       </c>
       <c r="O71" s="53">
         <v>1</v>
       </c>
       <c r="P71" s="29">
-        <f t="shared" si="0"/>
-        <v>16.100000000000001</v>
-      </c>
-      <c r="Q71" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="R71" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="T71">
-        <f>IF(AND(Q71="Nicht Gekauft", R71="Benötigt"), P71, 0)</f>
-        <v>16.100000000000001</v>
-      </c>
+        <f>N71*O71</f>
+        <v>5.54</v>
+      </c>
+      <c r="Q71" s="30"/>
+      <c r="R71" s="31"/>
+      <c r="S71" s="6"/>
       <c r="U71">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="50" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="B72" s="50" t="s">
-        <v>101</v>
+        <v>231</v>
       </c>
       <c r="C72" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="51" t="s">
-        <v>144</v>
+      <c r="D72" s="50" t="s">
+        <v>233</v>
       </c>
       <c r="E72" s="50" t="s">
-        <v>103</v>
+        <v>234</v>
       </c>
       <c r="F72" s="50"/>
       <c r="G72" s="50"/>
       <c r="H72" s="50"/>
       <c r="I72" s="54"/>
       <c r="J72" s="54" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="K72" s="54"/>
       <c r="L72" s="50" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
       <c r="M72" s="50" t="str">
         <f t="shared" si="8"/>
-        <v>Amazon</v>
+        <v>DigiKey</v>
       </c>
       <c r="N72" s="52">
-        <v>6.99</v>
+        <v>0.19</v>
       </c>
       <c r="O72" s="53">
         <v>1</v>
       </c>
       <c r="P72" s="33">
         <f>N72*O72</f>
-        <v>6.99</v>
+        <v>0.19</v>
       </c>
       <c r="Q72" s="34"/>
       <c r="R72" s="25"/>
+      <c r="S72" s="6"/>
       <c r="U72">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF72" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="73" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B73" s="50" t="s">
         <v>101</v>
@@ -6143,49 +6177,54 @@
         <v>71</v>
       </c>
       <c r="D73" s="51" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="E73" s="50" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="F73" s="50"/>
       <c r="G73" s="50"/>
       <c r="H73" s="50"/>
       <c r="I73" s="54"/>
       <c r="J73" s="54" t="s">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="K73" s="54"/>
       <c r="L73" s="50" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="M73" s="50" t="str">
         <f t="shared" si="8"/>
-        <v>RobotShop</v>
+        <v>DigiKey</v>
       </c>
       <c r="N73" s="52">
-        <v>9.33</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="O73" s="53">
         <v>1</v>
       </c>
       <c r="P73" s="29">
-        <f>N73*O73</f>
-        <v>9.33</v>
-      </c>
-      <c r="Q73" s="30"/>
-      <c r="R73" s="31"/>
+        <f t="shared" si="0"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q73" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="R73" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="T73">
+        <f>IF(AND(Q73="Nicht Gekauft", R73="Benötigt"), P73, 0)</f>
+        <v>16.100000000000001</v>
+      </c>
       <c r="U73">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF73" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="50" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B74" s="50" t="s">
         <v>101</v>
@@ -6194,35 +6233,35 @@
         <v>71</v>
       </c>
       <c r="D74" s="51" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E74" s="50" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="F74" s="50"/>
       <c r="G74" s="50"/>
       <c r="H74" s="50"/>
       <c r="I74" s="54"/>
       <c r="J74" s="54" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="K74" s="54"/>
       <c r="L74" s="50" t="s">
-        <v>153</v>
+        <v>259</v>
       </c>
       <c r="M74" s="50" t="str">
         <f t="shared" si="8"/>
-        <v>DigiKey</v>
+        <v>Amazon</v>
       </c>
       <c r="N74" s="52">
-        <v>3.39</v>
+        <v>6.99</v>
       </c>
       <c r="O74" s="53">
         <v>1</v>
       </c>
       <c r="P74" s="33">
         <f>N74*O74</f>
-        <v>3.39</v>
+        <v>6.99</v>
       </c>
       <c r="Q74" s="34"/>
       <c r="R74" s="25"/>
@@ -6231,77 +6270,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="50" t="s">
-        <v>57</v>
+        <v>143</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C75" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="50" t="s">
-        <v>59</v>
+        <v>101</v>
+      </c>
+      <c r="C75" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D75" s="51" t="s">
+        <v>146</v>
       </c>
       <c r="E75" s="50" t="s">
-        <v>60</v>
+        <v>147</v>
       </c>
       <c r="F75" s="50"/>
       <c r="G75" s="50"/>
       <c r="H75" s="50"/>
       <c r="I75" s="54"/>
       <c r="J75" s="54" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="K75" s="54"/>
       <c r="L75" s="50" t="s">
-        <v>258</v>
+        <v>149</v>
       </c>
       <c r="M75" s="50" t="str">
         <f t="shared" si="8"/>
-        <v>Amazon</v>
+        <v>RobotShop</v>
       </c>
       <c r="N75" s="52">
-        <v>16.13</v>
+        <v>9.33</v>
       </c>
       <c r="O75" s="53">
         <v>1</v>
       </c>
       <c r="P75" s="29">
-        <f t="shared" si="0"/>
-        <v>16.13</v>
-      </c>
-      <c r="Q75" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="R75" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="T75">
-        <f>IF(AND(Q75="Nicht Gekauft", R75="Benötigt"), P75, 0)</f>
-        <v>16.13</v>
-      </c>
+        <f>N75*O75</f>
+        <v>9.33</v>
+      </c>
+      <c r="Q75" s="30"/>
+      <c r="R75" s="31"/>
       <c r="U75">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AF75" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="76" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="50" t="s">
-        <v>61</v>
+        <v>150</v>
       </c>
       <c r="B76" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="C76" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="50" t="s">
-        <v>63</v>
+        <v>101</v>
+      </c>
+      <c r="C76" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" s="51" t="s">
+        <v>151</v>
       </c>
       <c r="E76" s="50" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
       <c r="F76" s="50"/>
       <c r="G76" s="50"/>
@@ -6312,86 +6346,86 @@
       </c>
       <c r="K76" s="54"/>
       <c r="L76" s="50" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="M76" s="50" t="str">
         <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N76" s="52">
-        <v>2.97</v>
+        <v>3.39</v>
       </c>
       <c r="O76" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P76" s="33">
-        <f t="shared" si="0"/>
-        <v>5.94</v>
-      </c>
-      <c r="Q76" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="R76" s="25" t="s">
-        <v>22</v>
-      </c>
+        <f>N76*O76</f>
+        <v>3.39</v>
+      </c>
+      <c r="Q76" s="34"/>
+      <c r="R76" s="25"/>
       <c r="U76">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="50" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B77" s="50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C77" s="50" t="s">
         <v>56</v>
       </c>
       <c r="D77" s="50" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E77" s="50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F77" s="50"/>
       <c r="G77" s="50"/>
       <c r="H77" s="50"/>
       <c r="I77" s="54"/>
       <c r="J77" s="54" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="K77" s="54"/>
       <c r="L77" s="50" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M77" s="50" t="str">
         <f t="shared" si="8"/>
-        <v>DigiKey</v>
+        <v>Amazon</v>
       </c>
       <c r="N77" s="52">
-        <v>5.92</v>
+        <v>16.13</v>
       </c>
       <c r="O77" s="53">
         <v>1</v>
       </c>
       <c r="P77" s="29">
         <f t="shared" si="0"/>
-        <v>5.92</v>
+        <v>16.13</v>
       </c>
       <c r="Q77" s="30" t="s">
         <v>21</v>
       </c>
       <c r="R77" s="31" t="s">
-        <v>22</v>
+        <v>108</v>
+      </c>
+      <c r="T77">
+        <f>IF(AND(Q77="Nicht Gekauft", R77="Benötigt"), P77, 0)</f>
+        <v>16.13</v>
       </c>
       <c r="U77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="50" t="s">
         <v>61</v>
       </c>
@@ -6402,7 +6436,7 @@
         <v>56</v>
       </c>
       <c r="D78" s="50" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E78" s="50" t="s">
         <v>64</v>
@@ -6416,302 +6450,440 @@
       </c>
       <c r="K78" s="54"/>
       <c r="L78" s="50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M78" s="50" t="str">
-        <f>HYPERLINK(L78,J78)</f>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N78" s="52">
-        <v>2.64</v>
+        <v>2.97</v>
       </c>
       <c r="O78" s="53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P78" s="33">
         <f t="shared" si="0"/>
-        <v>2.64</v>
+        <v>5.94</v>
       </c>
       <c r="Q78" s="34" t="s">
         <v>21</v>
       </c>
       <c r="R78" s="25" t="s">
         <v>22</v>
-      </c>
-      <c r="T78">
-        <f>IF(AND(Q78="Nicht Gekauft", R78="Benötigt"), P78, 0)</f>
-        <v>0</v>
       </c>
       <c r="U78">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="14"/>
-      <c r="K79" s="14"/>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="16"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="16"/>
-      <c r="Q79" s="17"/>
-    </row>
-    <row r="80" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P80" s="49"/>
-    </row>
-    <row r="81" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F81" s="5" t="s">
+    <row r="79" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D79" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E79" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="54"/>
+      <c r="J79" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="K79" s="54"/>
+      <c r="L79" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="M79" s="50" t="str">
+        <f t="shared" si="8"/>
+        <v>DigiKey</v>
+      </c>
+      <c r="N79" s="52">
+        <v>5.92</v>
+      </c>
+      <c r="O79" s="53">
+        <v>1</v>
+      </c>
+      <c r="P79" s="29">
+        <f t="shared" si="0"/>
+        <v>5.92</v>
+      </c>
+      <c r="Q79" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="R79" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="U79">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B80" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E80" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F80" s="50"/>
+      <c r="G80" s="50"/>
+      <c r="H80" s="50"/>
+      <c r="I80" s="54"/>
+      <c r="J80" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="K80" s="54"/>
+      <c r="L80" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="M80" s="50" t="str">
+        <f>HYPERLINK(L80,J80)</f>
+        <v>DigiKey</v>
+      </c>
+      <c r="N80" s="52">
+        <v>2.64</v>
+      </c>
+      <c r="O80" s="53">
+        <v>1</v>
+      </c>
+      <c r="P80" s="33">
+        <f t="shared" si="0"/>
+        <v>2.64</v>
+      </c>
+      <c r="Q80" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="R80" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="T80">
+        <f>IF(AND(Q80="Nicht Gekauft", R80="Benötigt"), P80, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U80">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="16"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="16"/>
+      <c r="Q81" s="17"/>
+    </row>
+    <row r="82" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P82" s="49"/>
+    </row>
+    <row r="83" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F83" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="G81" s="5" t="s">
+      <c r="G83" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F82" s="43" t="s">
+    <row r="84" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F84" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="G82" s="43" t="s">
+      <c r="G84" s="43" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="83" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F83" s="44">
-        <f>SUMPRODUCT(F2:F78, O2:O78, U2:U78)</f>
-        <v>6.7679999999999989</v>
-      </c>
-      <c r="G83" s="44" t="e" cm="1">
-        <f t="array" ref="G83">SUMPRODUCT((G2:G78=12)*(F2:F78)*(O2:O78)*(U2:U78))</f>
+    <row r="85" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F85" s="44">
+        <f>SUMPRODUCT(F2:F80, O2:O80, U2:U80)</f>
+        <v>4.7199999999999989</v>
+      </c>
+      <c r="G85" s="44" t="e" cm="1">
+        <f t="array" ref="G85">SUMPRODUCT((G2:G80=12)*(F2:F80)*(O2:O80)*(U2:U80))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H83" s="3"/>
-    </row>
-    <row r="84" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H84" s="3"/>
-    </row>
-    <row r="85" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G85" s="43" t="s">
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G87" s="43" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="86" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G86" s="44" t="e" cm="1">
-        <f t="array" ref="G86">SUMPRODUCT((G2:G78=5)*(F2:F78)*(O2:O78)*(U2:U78))</f>
+    <row r="88" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G88" s="44" t="e" cm="1">
+        <f t="array" ref="G88">SUMPRODUCT((G2:G80=5)*(F2:F80)*(O2:O80)*(U2:U80))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H86" s="3"/>
-    </row>
-    <row r="87" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H87" s="3"/>
-    </row>
-    <row r="88" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F88" s="5" t="s">
+      <c r="H88" s="3"/>
+    </row>
+    <row r="89" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H89" s="3"/>
+    </row>
+    <row r="90" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F90" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="G88" s="5" t="s">
+      <c r="G90" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="H88" s="3"/>
-    </row>
-    <row r="89" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F89" s="38" t="s">
+      <c r="H90" s="3"/>
+    </row>
+    <row r="91" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F91" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="G89" s="38" t="s">
+      <c r="G91" s="38" t="s">
         <v>269</v>
       </c>
-      <c r="H89" s="3"/>
-    </row>
-    <row r="90" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F90" s="39">
-        <f>F83*$F$93</f>
-        <v>10.151999999999997</v>
-      </c>
-      <c r="G90" s="39" t="e">
-        <f>G83*$F$93</f>
+      <c r="H91" s="3"/>
+    </row>
+    <row r="92" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F92" s="39">
+        <f>F85*$F$95</f>
+        <v>7.0799999999999983</v>
+      </c>
+      <c r="G92" s="39" t="e">
+        <f>G85*$F$95</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H90" s="3"/>
-      <c r="L90" s="7"/>
-      <c r="M90" s="7"/>
-    </row>
-    <row r="91" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H91" s="3"/>
-    </row>
-    <row r="92" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F92" s="41" t="s">
+      <c r="H92" s="3"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="7"/>
+    </row>
+    <row r="93" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H93" s="3"/>
+    </row>
+    <row r="94" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F94" s="41" t="s">
         <v>275</v>
       </c>
-      <c r="G92" s="38" t="s">
+      <c r="G94" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="H92" s="3"/>
-    </row>
-    <row r="93" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F93" s="42">
+      <c r="H94" s="3"/>
+    </row>
+    <row r="95" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F95" s="42">
         <v>1.5</v>
       </c>
-      <c r="G93" s="39" t="e">
-        <f>G86*$F$93</f>
+      <c r="G95" s="39" t="e">
+        <f>G88*$F$95</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H93" s="3"/>
-    </row>
-    <row r="94" spans="6:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H94" s="3"/>
-      <c r="I94" s="3" t="s">
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H96" s="3"/>
+      <c r="I96" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="95" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F95" s="5" t="s">
+    <row r="97" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F97" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="G95" s="5" t="s">
+      <c r="G97" s="5" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="96" spans="6:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F96" s="47">
-        <f>SUM(F2:F78)</f>
+    <row r="98" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F98" s="47">
+        <f>SUM(F2:F80)</f>
         <v>4.622399999999999</v>
       </c>
-      <c r="G96" s="46" t="s">
+      <c r="G98" s="46" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="97" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G97" s="48">
+    <row r="99" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G99" s="48">
         <v>3.04</v>
-      </c>
-    </row>
-    <row r="98" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F98" s="40"/>
-      <c r="G98" s="40"/>
-    </row>
-    <row r="99" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F99" s="40"/>
-      <c r="G99" s="45" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="100" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F100" s="40"/>
-      <c r="G100" s="47">
+      <c r="G100" s="40"/>
+    </row>
+    <row r="101" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F101" s="40"/>
+      <c r="G101" s="45" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="102" spans="6:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F102" s="40"/>
+      <c r="G102" s="47">
         <v>2.548</v>
-      </c>
-    </row>
-    <row r="102" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F102" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="103" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F103" t="s">
-        <v>285</v>
-      </c>
-      <c r="G103">
-        <v>8</v>
       </c>
     </row>
     <row r="104" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F104" t="s">
-        <v>286</v>
-      </c>
-      <c r="G104">
-        <v>5</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F105" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G105">
-        <v>0.05</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>286</v>
+      </c>
+      <c r="G106">
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F107" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="108" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F108" t="s">
-        <v>288</v>
-      </c>
-      <c r="G108" t="e">
-        <f>G103-G90</f>
-        <v>#VALUE!</v>
+        <v>287</v>
+      </c>
+      <c r="G107">
+        <v>0.05</v>
       </c>
     </row>
     <row r="109" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F109" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="110" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>288</v>
+      </c>
+      <c r="G110" t="e">
+        <f>G105-G92</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="111" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
         <v>289</v>
       </c>
-      <c r="G109" t="e">
-        <f>G104+G105-G93</f>
+      <c r="G111" t="e">
+        <f>G106+G107-G95</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="112" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F112" t="s">
+    <row r="114" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
         <v>329</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R78" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
+  <autoFilter ref="A1:R80" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
     <filterColumn colId="0">
       <filters blank="1">
-        <filter val="ACC1"/>
-        <filter val="ACC2"/>
         <filter val="ACC3"/>
-        <filter val="ACC4"/>
-        <filter val="BF1"/>
-        <filter val="BF2"/>
-        <filter val="BF2.1"/>
-        <filter val="BF3"/>
         <filter val="BF4"/>
         <filter val="BL"/>
-        <filter val="BP1"/>
         <filter val="BP2"/>
-        <filter val="F1"/>
         <filter val="F2"/>
-        <filter val="POW1"/>
         <filter val="POW2"/>
         <filter val="S1"/>
-        <filter val="S2"/>
-        <filter val="SP1"/>
         <filter val="SP2"/>
-        <filter val="SP3"/>
-        <filter val="ST1"/>
-        <filter val="ST2"/>
-        <filter val="ST3"/>
         <filter val="ST4"/>
-        <filter val="SV1"/>
         <filter val="SV2"/>
-        <filter val="TP1"/>
         <filter val="TP2"/>
-        <filter val="TP3"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{36C50999-9392-45D3-927D-2C21A30118D3}" filter="1" showAutoFilter="1" hiddenColumns="1">
+    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
+      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:R78" xr:uid="{B4F3BF44-7F35-4143-9930-25E8186FF7E9}">
+      <autoFilter ref="A1:R62" xr:uid="{DACF0EC9-E953-4566-81C6-E0B5C1F29F19}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="POW2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A1:R59" xr:uid="{5A177483-DA3F-4128-A022-84F0543D6468}"/>
+    </customSheetView>
+    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A1:R59" xr:uid="{BF617042-15E5-462F-9740-087C5A669362}"/>
+    </customSheetView>
+    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <autoFilter ref="A1:R60" xr:uid="{BCFD0613-FAA5-4F1E-8905-AC0D6DD8AAFE}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+      <autoFilter ref="A1:R78" xr:uid="{8B2E7D8C-ED53-44A7-AA2B-6543D1A4AD8C}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6729,12 +6901,12 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{B27C99E1-F194-4CDD-BEEF-0E7944A43981}" filter="1" showAutoFilter="1" hiddenColumns="1">
+    <customSheetView guid="{36C50999-9392-45D3-927D-2C21A30118D3}" filter="1" showAutoFilter="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
+      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:R78" xr:uid="{FBEFBE2B-D72E-4F13-947F-7414729BFF82}">
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+      <autoFilter ref="A1:R78" xr:uid="{E1F712C2-8EC8-436E-87AE-D6F619D55EE9}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6747,59 +6919,6 @@
             <filter val="SP2"/>
             <filter val="ST4"/>
             <filter val="SV2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{86D49B71-F0A7-4EDF-9F83-437E8F1DE26F}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1:U1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A1:R60" xr:uid="{EA93ABE8-2E41-4C2A-8766-8D8CA804B251}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A1:R59" xr:uid="{41BA9B40-8A1F-4113-8953-025FFA734C02}"/>
-    </customSheetView>
-    <customSheetView guid="{E3E09E1D-E21B-434F-8777-BA2F5DFE998D}" showAutoFilter="1" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-      <autoFilter ref="A1:R59" xr:uid="{D96542F2-6C6A-44BF-82CF-19E96D686E62}"/>
-    </customSheetView>
-    <customSheetView guid="{AD0CFDC5-A886-4774-8323-B873BC9D36B7}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-      <autoFilter ref="A1:R62" xr:uid="{D5AD703C-60F1-4B87-AFA2-FE08B386F63B}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="POW2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
             <filter val="TP2"/>
           </filters>
         </filterColumn>
@@ -6825,7 +6944,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q35 Q39:Q84 Q86:Q1048576">
+  <conditionalFormatting sqref="Q1:Q35 Q39:Q86 Q88:Q1048576">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Nicht Gekauft"</formula>
     </cfRule>
@@ -6841,7 +6960,7 @@
       <formula>"Gekauft"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R35 R39:R79">
+  <conditionalFormatting sqref="R2:R35 R39:R81">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Nicht benötigt"</formula>
     </cfRule>
@@ -6849,43 +6968,43 @@
       <formula>"Benötigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R39:R79 R2:R35" xr:uid="{DF639F38-DCBF-4FB0-9016-BE70B5447265}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R39:R81 R2:R35" xr:uid="{DF639F38-DCBF-4FB0-9016-BE70B5447265}">
       <formula1>"Benötigt,Nicht benötigt"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q39:Q79 Q2:Q35" xr:uid="{BB82D80E-695D-4A38-A148-48463DFE8321}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q39:Q81 Q2:Q35" xr:uid="{BB82D80E-695D-4A38-A148-48463DFE8321}">
       <formula1>"Gekauft,Nicht Gekauft"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId7" xr:uid="{134576B2-6870-47F8-80B5-95CA9B97F9E2}"/>
     <hyperlink ref="L58" r:id="rId8" xr:uid="{F3AD9EFC-A933-40C0-B3D6-105AE81F974F}"/>
-    <hyperlink ref="L59" r:id="rId9" xr:uid="{0B081703-43B3-49C1-ABA0-60C83F319C14}"/>
-    <hyperlink ref="L60" r:id="rId10" xr:uid="{A386B0E7-0270-440F-94E8-1A585C273E01}"/>
+    <hyperlink ref="L60" r:id="rId9" xr:uid="{0B081703-43B3-49C1-ABA0-60C83F319C14}"/>
+    <hyperlink ref="L61" r:id="rId10" xr:uid="{A386B0E7-0270-440F-94E8-1A585C273E01}"/>
     <hyperlink ref="L39" r:id="rId11" xr:uid="{6E8ED221-C460-4F2D-A839-674D0DD8E486}"/>
-    <hyperlink ref="L76" r:id="rId12" xr:uid="{9A0B0992-EB9B-485C-8743-AB5373B961C2}"/>
-    <hyperlink ref="L78" r:id="rId13" xr:uid="{B67FB571-1B87-4184-A2B3-AF411BD87D35}"/>
-    <hyperlink ref="L64" r:id="rId14" xr:uid="{57963C92-CE56-4D91-B1F1-7FA05F5BC3A8}"/>
-    <hyperlink ref="L63" r:id="rId15" xr:uid="{9D795571-0999-43FF-9A1F-496FF99C86C0}"/>
-    <hyperlink ref="L65" r:id="rId16" xr:uid="{8465788D-FDE3-460C-960F-435D2FB5F396}"/>
+    <hyperlink ref="L78" r:id="rId12" xr:uid="{9A0B0992-EB9B-485C-8743-AB5373B961C2}"/>
+    <hyperlink ref="L80" r:id="rId13" xr:uid="{B67FB571-1B87-4184-A2B3-AF411BD87D35}"/>
+    <hyperlink ref="L66" r:id="rId14" xr:uid="{57963C92-CE56-4D91-B1F1-7FA05F5BC3A8}"/>
+    <hyperlink ref="L65" r:id="rId15" xr:uid="{9D795571-0999-43FF-9A1F-496FF99C86C0}"/>
+    <hyperlink ref="L67" r:id="rId16" xr:uid="{8465788D-FDE3-460C-960F-435D2FB5F396}"/>
     <hyperlink ref="L10" r:id="rId17" xr:uid="{A9D6150D-3C06-4D81-AD60-047F4F409296}"/>
     <hyperlink ref="L11" r:id="rId18" xr:uid="{411A7094-1AC1-4084-ABE4-5C0060EC1A2D}"/>
     <hyperlink ref="L12" r:id="rId19" xr:uid="{3DDB6C5A-7DB3-4C65-B604-D02293535F49}"/>
     <hyperlink ref="L7" r:id="rId20" xr:uid="{56E44BCE-942A-4E32-8574-907151789664}"/>
-    <hyperlink ref="L71" r:id="rId21" xr:uid="{D632E27D-8B4B-473B-9951-117DBC2C36E0}"/>
+    <hyperlink ref="L73" r:id="rId21" xr:uid="{D632E27D-8B4B-473B-9951-117DBC2C36E0}"/>
     <hyperlink ref="L3" r:id="rId22" xr:uid="{C49F6822-A4DD-42C2-B3BF-0381D137937C}"/>
     <hyperlink ref="L5" r:id="rId23" xr:uid="{BF0FEABB-4850-4BC5-A11D-D889C6B926FD}"/>
     <hyperlink ref="L8" r:id="rId24" xr:uid="{21389653-C0FE-46E1-B136-04B9A0DE28C5}"/>
-    <hyperlink ref="L66" r:id="rId25" xr:uid="{1242A3DC-9FDC-4C47-9270-1B4A92E75E73}"/>
+    <hyperlink ref="L68" r:id="rId25" xr:uid="{1242A3DC-9FDC-4C47-9270-1B4A92E75E73}"/>
     <hyperlink ref="L36" r:id="rId26" xr:uid="{3ED73B15-E49B-4E21-BF8D-06828BFBADB2}"/>
     <hyperlink ref="L9" r:id="rId27" xr:uid="{E62708AD-A075-4D9D-9BC8-2CBD617B66EE}"/>
     <hyperlink ref="L37" r:id="rId28" xr:uid="{488C7B18-56E0-4061-83E3-FAA678922DF9}"/>
     <hyperlink ref="L43" r:id="rId29" xr:uid="{02A8F53B-7033-433E-97B4-37D43B10ABDE}"/>
-    <hyperlink ref="K61" r:id="rId30" display="https://www.samtec.com/products/hle-107-02-l-dv" xr:uid="{AF2D4394-67CE-4447-B187-DA356AB0AFD4}"/>
-    <hyperlink ref="L61" r:id="rId31" xr:uid="{3CAA47B9-FD6F-4B23-A59B-6E4BF51797D7}"/>
+    <hyperlink ref="K62" r:id="rId30" display="https://www.samtec.com/products/hle-107-02-l-dv" xr:uid="{AF2D4394-67CE-4447-B187-DA356AB0AFD4}"/>
+    <hyperlink ref="L62" r:id="rId31" xr:uid="{3CAA47B9-FD6F-4B23-A59B-6E4BF51797D7}"/>
     <hyperlink ref="L21" r:id="rId32" xr:uid="{8FDFC79B-94E5-4C68-84E1-D5C8679D313C}"/>
     <hyperlink ref="L22" r:id="rId33" xr:uid="{3CB626FF-165C-4A7E-A7FE-D41E681D5EC5}"/>
-    <hyperlink ref="L68" r:id="rId34" xr:uid="{B06D0A87-6477-4382-AFA7-5ACA40E62DA0}"/>
+    <hyperlink ref="L70" r:id="rId34" xr:uid="{B06D0A87-6477-4382-AFA7-5ACA40E62DA0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>

</xml_diff>

<commit_message>
struktur verbessert, wireviz zu pngs exportiert
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
+++ b/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E650044-5144-4184-B1F9-43555C240495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F960C3C-67C3-492C-A72B-95E82004F3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,13 +37,13 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Strombudget_Foto" guid="{E35F6895-3697-4266-BC90-C5022F400E13}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
+    <customWorkbookView name="Default" guid="{4300A442-0A40-4FB1-A9F3-2AB99D5A4993}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
+    <customWorkbookView name="Strombudget" guid="{0C0F82AC-DC21-4B4A-94AC-E96E30BF52DE}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
+    <customWorkbookView name="Schaltplan" guid="{3411E606-57DF-4B4E-942D-8A879EBC3FAD}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
+    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
+    <customWorkbookView name="Anforderungen_prompt" guid="{1253E34A-3A91-496E-8486-95C1D21A2085}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
     <customWorkbookView name="Stueckliste_ansicht_export" guid="{2376F375-2D91-4AB8-9819-CC132C3118EA}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Anforderungen_prompt" guid="{1253E34A-3A91-496E-8486-95C1D21A2085}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
-    <customWorkbookView name="Bauteil hinzufügen" guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" maximized="1" xWindow="2552" yWindow="192" windowWidth="1936" windowHeight="1048" activeSheetId="5"/>
-    <customWorkbookView name="Schaltplan" guid="{3411E606-57DF-4B4E-942D-8A879EBC3FAD}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
-    <customWorkbookView name="Strombudget" guid="{0C0F82AC-DC21-4B4A-94AC-E96E30BF52DE}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
-    <customWorkbookView name="Default" guid="{4300A442-0A40-4FB1-A9F3-2AB99D5A4993}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
-    <customWorkbookView name="Strombudget_Foto" guid="{E35F6895-3697-4266-BC90-C5022F400E13}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="2576" windowHeight="1408" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1978,6 +1978,9 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2001,9 +2004,6 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2401,8 +2401,8 @@
   <dimension ref="A1:AM105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO19" sqref="AO19"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2498,18 +2498,18 @@
       <c r="U1" t="s">
         <v>223</v>
       </c>
-      <c r="X1" s="59" t="s">
+      <c r="X1" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" s="60"/>
+      <c r="Y1" s="61"/>
       <c r="Z1" s="11">
         <f>SUMIFS(P44:P71,Q44:Q71, "Nicht Gekauft",R44:R71,"Benötigt")</f>
         <v>19.07</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" s="58"/>
+      <c r="AC1" s="59"/>
       <c r="AD1" s="10">
         <f>SUM(P3:P71)</f>
         <v>367.67999999999984</v>
@@ -2547,7 +2547,7 @@
         <v>382</v>
       </c>
       <c r="M2" s="48" t="str">
-        <f>HYPERLINK(L2,J2)</f>
+        <f t="shared" ref="M2:M11" si="0">HYPERLINK(L2,J2)</f>
         <v>DigikKey</v>
       </c>
       <c r="N2" s="50">
@@ -2557,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="29">
-        <f t="shared" ref="P2:P6" si="0">N2*O2</f>
+        <f t="shared" ref="P2:P6" si="1">N2*O2</f>
         <v>33.369999999999997</v>
       </c>
       <c r="Q2" s="30"/>
@@ -2593,7 +2593,7 @@
         <v>165</v>
       </c>
       <c r="M3" s="48" t="str">
-        <f>HYPERLINK(L3,J3)</f>
+        <f t="shared" si="0"/>
         <v>DigiKey</v>
       </c>
       <c r="N3" s="50">
@@ -2603,13 +2603,13 @@
         <v>1</v>
       </c>
       <c r="P3" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="Q3" s="30"/>
       <c r="R3" s="31"/>
       <c r="U3">
-        <f t="shared" ref="U3:U28" si="1">SUBTOTAL(103, G3)</f>
+        <f t="shared" ref="U3:U28" si="2">SUBTOTAL(103, G3)</f>
         <v>1</v>
       </c>
     </row>
@@ -2643,7 +2643,7 @@
         <v>167</v>
       </c>
       <c r="M4" s="48" t="str">
-        <f>HYPERLINK(L4,J4)</f>
+        <f t="shared" si="0"/>
         <v>DigiKey</v>
       </c>
       <c r="N4" s="50">
@@ -2653,13 +2653,13 @@
         <v>1</v>
       </c>
       <c r="P4" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="Q4" s="33"/>
       <c r="R4" s="25"/>
       <c r="U4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AG4" t="s">
@@ -2692,7 +2692,7 @@
         <v>202</v>
       </c>
       <c r="M5" s="48" t="str">
-        <f>HYPERLINK(L5,J5)</f>
+        <f t="shared" si="0"/>
         <v>DigiKey</v>
       </c>
       <c r="N5" s="50">
@@ -2702,13 +2702,13 @@
         <v>1</v>
       </c>
       <c r="P5" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41</v>
       </c>
       <c r="Q5" s="33"/>
       <c r="R5" s="25"/>
       <c r="U5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF5" t="s">
@@ -2741,7 +2741,7 @@
         <v>204</v>
       </c>
       <c r="M6" s="48" t="str">
-        <f>HYPERLINK(L6,J6)</f>
+        <f t="shared" si="0"/>
         <v>DigiKey</v>
       </c>
       <c r="N6" s="50">
@@ -2751,13 +2751,13 @@
         <v>1</v>
       </c>
       <c r="P6" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23</v>
       </c>
       <c r="Q6" s="30"/>
       <c r="R6" s="31"/>
       <c r="U6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF6" t="s">
@@ -2790,7 +2790,7 @@
         <v>20</v>
       </c>
       <c r="M7" s="48" t="str">
-        <f>HYPERLINK(L7,J7)</f>
+        <f t="shared" si="0"/>
         <v>Stepperonline</v>
       </c>
       <c r="N7" s="50">
@@ -2800,7 +2800,7 @@
         <v>1</v>
       </c>
       <c r="P7" s="29">
-        <f>N7*O7</f>
+        <f t="shared" ref="P7:P15" si="3">N7*O7</f>
         <v>9.91</v>
       </c>
       <c r="Q7" s="30" t="s">
@@ -2814,13 +2814,13 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <f>SUBTOTAL(103, G7)</f>
+        <f t="shared" ref="U7:U15" si="4">SUBTOTAL(103, G7)</f>
         <v>0</v>
       </c>
-      <c r="X7" s="63" t="s">
+      <c r="X7" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="Y7" s="64"/>
+      <c r="Y7" s="65"/>
       <c r="Z7" s="12">
         <f>SUBTOTAL(9,P1:P71)</f>
         <v>221.24999999999994</v>
@@ -2861,7 +2861,7 @@
         <v>27</v>
       </c>
       <c r="M8" s="48" t="str">
-        <f>HYPERLINK(L8,J8)</f>
+        <f t="shared" si="0"/>
         <v>AZ-Delivery</v>
       </c>
       <c r="N8" s="50">
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="32">
-        <f>N8*O8</f>
+        <f t="shared" si="3"/>
         <v>6.99</v>
       </c>
       <c r="Q8" s="33" t="s">
@@ -2881,7 +2881,7 @@
         <v>81</v>
       </c>
       <c r="U8">
-        <f>SUBTOTAL(103, G8)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X8" s="34"/>
@@ -2923,7 +2923,7 @@
         <v>91</v>
       </c>
       <c r="M9" s="48" t="str">
-        <f>HYPERLINK(L9,J9)</f>
+        <f t="shared" si="0"/>
         <v>3D-Jake</v>
       </c>
       <c r="N9" s="50">
@@ -2933,19 +2933,19 @@
         <v>1</v>
       </c>
       <c r="P9" s="29">
-        <f>N9*O9</f>
+        <f t="shared" si="3"/>
         <v>6.99</v>
       </c>
       <c r="Q9" s="30"/>
       <c r="R9" s="31"/>
       <c r="U9">
-        <f>SUBTOTAL(103, G9)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X9" s="61" t="s">
+      <c r="X9" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="Y9" s="62"/>
+      <c r="Y9" s="63"/>
       <c r="Z9" s="9">
         <f>SUBTOTAL(9,T1:T71)</f>
         <v>14.030000000000001</v>
@@ -2981,7 +2981,7 @@
         <v>32</v>
       </c>
       <c r="M10" s="48" t="str">
-        <f>HYPERLINK(L10,J10)</f>
+        <f t="shared" si="0"/>
         <v>AZ-Delivery</v>
       </c>
       <c r="N10" s="50">
@@ -2991,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="P10" s="32">
-        <f>N10*O10</f>
+        <f t="shared" si="3"/>
         <v>6.99</v>
       </c>
       <c r="Q10" s="33" t="s">
@@ -3005,7 +3005,7 @@
         <v>6.99</v>
       </c>
       <c r="U10">
-        <f>SUBTOTAL(103, G10)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF10" t="s">
@@ -3044,7 +3044,7 @@
         <v>217</v>
       </c>
       <c r="M11" s="48" t="str">
-        <f>HYPERLINK(L11,J11)</f>
+        <f t="shared" si="0"/>
         <v>3D-Jake</v>
       </c>
       <c r="N11" s="50">
@@ -3054,7 +3054,7 @@
         <v>1</v>
       </c>
       <c r="P11" s="32">
-        <f>N11*O11</f>
+        <f t="shared" si="3"/>
         <v>39.99</v>
       </c>
       <c r="Q11" s="33" t="s">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="R11" s="25"/>
       <c r="U11">
-        <f>SUBTOTAL(103, G11)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AF11" t="s">
@@ -3097,7 +3097,7 @@
         <v>77</v>
       </c>
       <c r="M12" s="48" t="str">
-        <f t="shared" ref="M12:M15" si="2">HYPERLINK(L12,J12)</f>
+        <f t="shared" ref="M12:M15" si="5">HYPERLINK(L12,J12)</f>
         <v>DigiKey</v>
       </c>
       <c r="N12" s="50">
@@ -3107,7 +3107,7 @@
         <v>1</v>
       </c>
       <c r="P12" s="29">
-        <f>N12*O12</f>
+        <f t="shared" si="3"/>
         <v>16.100000000000001</v>
       </c>
       <c r="Q12" s="30" t="s">
@@ -3121,7 +3121,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="U12">
-        <f>SUBTOTAL(103, G12)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3153,7 +3153,7 @@
         <v>211</v>
       </c>
       <c r="M13" s="48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Amazon</v>
       </c>
       <c r="N13" s="50">
@@ -3163,13 +3163,13 @@
         <v>1</v>
       </c>
       <c r="P13" s="32">
-        <f>N13*O13</f>
+        <f t="shared" si="3"/>
         <v>6.99</v>
       </c>
       <c r="Q13" s="33"/>
       <c r="R13" s="25"/>
       <c r="U13">
-        <f>SUBTOTAL(103, G13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3201,7 +3201,7 @@
         <v>377</v>
       </c>
       <c r="M14" s="48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>AZ-Delivery</v>
       </c>
       <c r="N14" s="50">
@@ -3211,13 +3211,13 @@
         <v>1</v>
       </c>
       <c r="P14" s="29">
-        <f>N14*O14</f>
+        <f t="shared" si="3"/>
         <v>5.99</v>
       </c>
       <c r="Q14" s="30"/>
       <c r="R14" s="31"/>
       <c r="U14">
-        <f>SUBTOTAL(103, G14)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF14" t="s">
@@ -3252,7 +3252,7 @@
         <v>110</v>
       </c>
       <c r="M15" s="48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>DigiKey</v>
       </c>
       <c r="N15" s="50">
@@ -3262,13 +3262,13 @@
         <v>1</v>
       </c>
       <c r="P15" s="32">
-        <f>N15*O15</f>
+        <f t="shared" si="3"/>
         <v>3.39</v>
       </c>
       <c r="Q15" s="33"/>
       <c r="R15" s="25"/>
       <c r="U15">
-        <f>SUBTOTAL(103, G15)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3305,7 +3305,7 @@
         <v>73</v>
       </c>
       <c r="M16" s="48" t="str">
-        <f t="shared" ref="M16:M71" si="3">HYPERLINK(L16,J16)</f>
+        <f t="shared" ref="M16:M71" si="6">HYPERLINK(L16,J16)</f>
         <v>Amazon</v>
       </c>
       <c r="N16" s="50">
@@ -3315,7 +3315,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="32">
-        <f t="shared" ref="P16:P71" si="4">N16*O16</f>
+        <f t="shared" ref="P16:P71" si="7">N16*O16</f>
         <v>34.119999999999997</v>
       </c>
       <c r="Q16" s="30" t="s">
@@ -3329,7 +3329,7 @@
         <v>34.119999999999997</v>
       </c>
       <c r="U16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3365,7 +3365,7 @@
         <v>92</v>
       </c>
       <c r="M17" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N17" s="50">
@@ -3375,7 +3375,7 @@
         <v>2</v>
       </c>
       <c r="P17" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13.46</v>
       </c>
       <c r="Q17" s="33" t="s">
@@ -3383,7 +3383,7 @@
       </c>
       <c r="R17" s="25"/>
       <c r="U17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AF17" t="s">
@@ -3422,7 +3422,7 @@
         <v>96</v>
       </c>
       <c r="M18" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N18" s="50">
@@ -3432,7 +3432,7 @@
         <v>2</v>
       </c>
       <c r="P18" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>14.8</v>
       </c>
       <c r="Q18" s="30" t="s">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="R18" s="31"/>
       <c r="U18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3455,7 +3455,7 @@
       <c r="D19" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="E19" s="57" t="s">
         <v>390</v>
       </c>
       <c r="F19" s="48"/>
@@ -3472,7 +3472,7 @@
         <v>387</v>
       </c>
       <c r="M19" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N19" s="50">
@@ -3482,7 +3482,7 @@
         <v>4</v>
       </c>
       <c r="P19" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="Q19" s="30"/>
@@ -3679,7 +3679,7 @@
         <v>193</v>
       </c>
       <c r="M23" s="48" t="str">
-        <f t="shared" ref="M23:M34" si="5">HYPERLINK(L23,J23)</f>
+        <f t="shared" ref="M23:M34" si="8">HYPERLINK(L23,J23)</f>
         <v>DigiKey</v>
       </c>
       <c r="N23" s="50">
@@ -3689,13 +3689,13 @@
         <v>1</v>
       </c>
       <c r="P23" s="29">
-        <f t="shared" ref="P23:P24" si="6">N23*O23</f>
+        <f t="shared" ref="P23:P24" si="9">N23*O23</f>
         <v>5.79</v>
       </c>
       <c r="Q23" s="30"/>
       <c r="R23" s="31"/>
       <c r="U23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3727,7 +3727,7 @@
         <v>196</v>
       </c>
       <c r="M24" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N24" s="50">
@@ -3737,13 +3737,13 @@
         <v>1</v>
       </c>
       <c r="P24" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.1399999999999997</v>
       </c>
       <c r="Q24" s="33"/>
       <c r="R24" s="25"/>
       <c r="U24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3779,7 +3779,7 @@
         <v>230</v>
       </c>
       <c r="M25" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N25" s="50">
@@ -3789,13 +3789,13 @@
         <v>1</v>
       </c>
       <c r="P25" s="32">
-        <f t="shared" ref="P25:P26" si="7">N25*O25</f>
+        <f t="shared" ref="P25:P26" si="10">N25*O25</f>
         <v>2.34</v>
       </c>
       <c r="Q25" s="30"/>
       <c r="R25" s="31"/>
       <c r="U25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AF25" t="s">
@@ -3836,7 +3836,7 @@
         <v>233</v>
       </c>
       <c r="M26" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N26" s="50">
@@ -3846,13 +3846,13 @@
         <v>1</v>
       </c>
       <c r="P26" s="32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.17</v>
       </c>
       <c r="Q26" s="33"/>
       <c r="R26" s="25"/>
       <c r="U26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF26" t="s">
@@ -3891,7 +3891,7 @@
         <v>268</v>
       </c>
       <c r="M27" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N27" s="50">
@@ -3901,13 +3901,13 @@
         <v>1</v>
       </c>
       <c r="P27" s="29">
-        <f t="shared" ref="P27:P32" si="8">N27*O27</f>
+        <f t="shared" ref="P27:P32" si="11">N27*O27</f>
         <v>1.78</v>
       </c>
       <c r="Q27" s="30"/>
       <c r="R27" s="31"/>
       <c r="U27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF27" t="s">
@@ -3943,7 +3943,7 @@
         <v>272</v>
       </c>
       <c r="M28" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N28" s="50">
@@ -3953,13 +3953,13 @@
         <v>1</v>
       </c>
       <c r="P28" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95</v>
       </c>
       <c r="Q28" s="30"/>
       <c r="R28" s="31"/>
       <c r="U28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF28" t="s">
@@ -3995,7 +3995,7 @@
         <v>179</v>
       </c>
       <c r="M29" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N29" s="50">
@@ -4005,7 +4005,7 @@
         <v>1</v>
       </c>
       <c r="P29" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.56</v>
       </c>
       <c r="Q29" s="33"/>
@@ -4044,7 +4044,7 @@
         <v>175</v>
       </c>
       <c r="M30" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N30" s="50">
@@ -4054,7 +4054,7 @@
         <v>1</v>
       </c>
       <c r="P30" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47</v>
       </c>
       <c r="Q30" s="30"/>
@@ -4093,7 +4093,7 @@
         <v>158</v>
       </c>
       <c r="M31" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Digikey</v>
       </c>
       <c r="N31" s="50">
@@ -4103,7 +4103,7 @@
         <v>2</v>
       </c>
       <c r="P31" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.6</v>
       </c>
       <c r="Q31" s="33"/>
@@ -4144,7 +4144,7 @@
         <v>243</v>
       </c>
       <c r="M32" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N32" s="50">
@@ -4154,7 +4154,7 @@
         <v>1</v>
       </c>
       <c r="P32" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.3</v>
       </c>
       <c r="Q32" s="33"/>
@@ -4186,7 +4186,7 @@
         <v>184</v>
       </c>
       <c r="M33" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N33" s="50">
@@ -4196,7 +4196,7 @@
         <v>2</v>
       </c>
       <c r="P33" s="29">
-        <f t="shared" ref="P33:P34" si="9">N33*O33</f>
+        <f t="shared" ref="P33:P34" si="12">N33*O33</f>
         <v>5.82</v>
       </c>
       <c r="Q33" s="30"/>
@@ -4239,7 +4239,7 @@
         <v>170</v>
       </c>
       <c r="M34" s="48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>DigiKey</v>
       </c>
       <c r="N34" s="50">
@@ -4249,7 +4249,7 @@
         <v>1</v>
       </c>
       <c r="P34" s="29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="Q34" s="30"/>
@@ -4307,7 +4307,7 @@
       <c r="Q35" s="28"/>
       <c r="R35" s="28"/>
       <c r="U35">
-        <f t="shared" ref="U35:U36" si="10">SUBTOTAL(103, G35)</f>
+        <f t="shared" ref="U35:U36" si="13">SUBTOTAL(103, G35)</f>
         <v>0</v>
       </c>
       <c r="AF35" t="s">
@@ -4359,7 +4359,7 @@
       <c r="Q36" s="28"/>
       <c r="R36" s="28"/>
       <c r="U36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -4393,7 +4393,7 @@
         <v>128</v>
       </c>
       <c r="M37" s="48" t="str">
-        <f t="shared" ref="M37:M43" si="11">HYPERLINK(L37,J37)</f>
+        <f t="shared" ref="M37:M43" si="14">HYPERLINK(L37,J37)</f>
         <v>DigiKey</v>
       </c>
       <c r="N37" s="50">
@@ -4410,7 +4410,7 @@
       <c r="R37" s="25"/>
       <c r="S37" s="8"/>
       <c r="U37">
-        <f t="shared" ref="U37:U42" si="12">SUBTOTAL(103, G37)</f>
+        <f t="shared" ref="U37:U42" si="15">SUBTOTAL(103, G37)</f>
         <v>0</v>
       </c>
     </row>
@@ -4442,7 +4442,7 @@
         <v>139</v>
       </c>
       <c r="M38" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>DigiKey</v>
       </c>
       <c r="N38" s="50">
@@ -4499,7 +4499,7 @@
         <v>131</v>
       </c>
       <c r="M39" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>DigiKey</v>
       </c>
       <c r="N39" s="50">
@@ -4509,14 +4509,14 @@
         <v>1</v>
       </c>
       <c r="P39" s="32">
-        <f t="shared" ref="P39:P41" si="13">N39*O39</f>
+        <f t="shared" ref="P39:P41" si="16">N39*O39</f>
         <v>0.82</v>
       </c>
       <c r="Q39" s="33"/>
       <c r="R39" s="25"/>
       <c r="S39" s="8"/>
       <c r="U39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4548,7 +4548,7 @@
         <v>144</v>
       </c>
       <c r="M40" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>DigiKey</v>
       </c>
       <c r="N40" s="50">
@@ -4558,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="P40" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.94</v>
       </c>
       <c r="Q40" s="30"/>
@@ -4606,7 +4606,7 @@
         <v>149</v>
       </c>
       <c r="M41" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>DigiKey</v>
       </c>
       <c r="N41" s="50">
@@ -4616,14 +4616,14 @@
         <v>1</v>
       </c>
       <c r="P41" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1.33</v>
       </c>
       <c r="Q41" s="33"/>
       <c r="R41" s="25"/>
       <c r="S41" s="8"/>
       <c r="U41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4655,7 +4655,7 @@
         <v>153</v>
       </c>
       <c r="M42" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>DigiKey</v>
       </c>
       <c r="N42" s="50">
@@ -4671,7 +4671,7 @@
       <c r="Q42" s="30"/>
       <c r="R42" s="31"/>
       <c r="U42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4703,7 +4703,7 @@
         <v>361</v>
       </c>
       <c r="M43" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>DigiKey</v>
       </c>
       <c r="N43" s="50">
@@ -4756,7 +4756,7 @@
         <v>61</v>
       </c>
       <c r="M44" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N44" s="50">
@@ -4766,7 +4766,7 @@
         <v>3</v>
       </c>
       <c r="P44" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.0699999999999998</v>
       </c>
       <c r="Q44" s="33" t="s">
@@ -4780,7 +4780,7 @@
         <v>0</v>
       </c>
       <c r="U44">
-        <f t="shared" ref="U44:U52" si="14">SUBTOTAL(103, G44)</f>
+        <f t="shared" ref="U44:U52" si="17">SUBTOTAL(103, G44)</f>
         <v>0</v>
       </c>
     </row>
@@ -4814,7 +4814,7 @@
         <v>64</v>
       </c>
       <c r="M45" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N45" s="50">
@@ -4824,7 +4824,7 @@
         <v>9</v>
       </c>
       <c r="P45" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.7700000000000005</v>
       </c>
       <c r="Q45" s="30" t="s">
@@ -4838,7 +4838,7 @@
         <v>0</v>
       </c>
       <c r="U45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4872,7 +4872,7 @@
         <v>67</v>
       </c>
       <c r="M46" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N46" s="50">
@@ -4882,7 +4882,7 @@
         <v>5</v>
       </c>
       <c r="P46" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>3.4499999999999997</v>
       </c>
       <c r="Q46" s="33" t="s">
@@ -4896,7 +4896,7 @@
         <v>0</v>
       </c>
       <c r="U46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4930,7 +4930,7 @@
         <v>212</v>
       </c>
       <c r="M47" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Amazon</v>
       </c>
       <c r="N47" s="50">
@@ -4940,7 +4940,7 @@
         <v>1</v>
       </c>
       <c r="P47" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>17.14</v>
       </c>
       <c r="Q47" s="30" t="s">
@@ -4954,7 +4954,7 @@
         <v>0</v>
       </c>
       <c r="U47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4988,7 +4988,7 @@
         <v>214</v>
       </c>
       <c r="M48" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Amazon</v>
       </c>
       <c r="N48" s="50">
@@ -4998,13 +4998,13 @@
         <v>1</v>
       </c>
       <c r="P48" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.0500000000000007</v>
       </c>
       <c r="Q48" s="33"/>
       <c r="R48" s="25"/>
       <c r="U48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5038,7 +5038,7 @@
         <v>213</v>
       </c>
       <c r="M49" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Amazon</v>
       </c>
       <c r="N49" s="50">
@@ -5048,7 +5048,7 @@
         <v>1</v>
       </c>
       <c r="P49" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.55</v>
       </c>
       <c r="Q49" s="30" t="s">
@@ -5063,7 +5063,7 @@
         <v>7.55</v>
       </c>
       <c r="U49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5095,7 +5095,7 @@
         <v>111</v>
       </c>
       <c r="M50" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N50" s="50">
@@ -5105,14 +5105,14 @@
         <v>1</v>
       </c>
       <c r="P50" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.22</v>
       </c>
       <c r="Q50" s="33"/>
       <c r="R50" s="25"/>
       <c r="S50" s="8"/>
       <c r="U50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF50" t="s">
@@ -5147,7 +5147,7 @@
         <v>121</v>
       </c>
       <c r="M51" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N51" s="50">
@@ -5157,14 +5157,14 @@
         <v>4</v>
       </c>
       <c r="P51" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.72</v>
       </c>
       <c r="Q51" s="30"/>
       <c r="R51" s="31"/>
       <c r="S51" s="8"/>
       <c r="U51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF51" t="s">
@@ -5199,7 +5199,7 @@
         <v>122</v>
       </c>
       <c r="M52" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N52" s="50">
@@ -5209,14 +5209,14 @@
         <v>2</v>
       </c>
       <c r="P52" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="Q52" s="33"/>
       <c r="R52" s="25"/>
       <c r="S52" s="8"/>
       <c r="U52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF52" t="s">
@@ -5253,7 +5253,7 @@
         <v>254</v>
       </c>
       <c r="M53" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N53" s="50">
@@ -5263,7 +5263,7 @@
         <v>1</v>
       </c>
       <c r="P53" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.78</v>
       </c>
       <c r="Q53" s="33"/>
@@ -5310,7 +5310,7 @@
         <v>1</v>
       </c>
       <c r="P54" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.73</v>
       </c>
       <c r="Q54" s="33"/>
@@ -5347,7 +5347,7 @@
         <v>256</v>
       </c>
       <c r="M55" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N55" s="50">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="O55" s="51"/>
       <c r="P55" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q55" s="33"/>
@@ -5392,7 +5392,7 @@
         <v>257</v>
       </c>
       <c r="M56" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N56" s="50">
@@ -5402,7 +5402,7 @@
         <v>1</v>
       </c>
       <c r="P56" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.21</v>
       </c>
       <c r="Q56" s="33"/>
@@ -5439,7 +5439,7 @@
         <v>258</v>
       </c>
       <c r="M57" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N57" s="50">
@@ -5449,7 +5449,7 @@
         <v>1</v>
       </c>
       <c r="P57" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="Q57" s="33"/>
@@ -5486,7 +5486,7 @@
         <v>259</v>
       </c>
       <c r="M58" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N58" s="50">
@@ -5496,7 +5496,7 @@
         <v>1</v>
       </c>
       <c r="P58" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
       <c r="Q58" s="33"/>
@@ -5535,7 +5535,7 @@
         <v>265</v>
       </c>
       <c r="M59" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N59" s="50">
@@ -5545,14 +5545,14 @@
         <v>1</v>
       </c>
       <c r="P59" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.24</v>
       </c>
       <c r="Q59" s="33"/>
       <c r="R59" s="25"/>
       <c r="S59" s="8"/>
       <c r="U59">
-        <f t="shared" ref="U59:U63" si="15">SUBTOTAL(103, G59)</f>
+        <f t="shared" ref="U59:U63" si="18">SUBTOTAL(103, G59)</f>
         <v>0</v>
       </c>
     </row>
@@ -5586,7 +5586,7 @@
         <v>263</v>
       </c>
       <c r="M60" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N60" s="50">
@@ -5596,14 +5596,14 @@
         <v>3</v>
       </c>
       <c r="P60" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.96</v>
       </c>
       <c r="Q60" s="33"/>
       <c r="R60" s="25"/>
       <c r="S60" s="8"/>
       <c r="U60">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
         <v>263</v>
       </c>
       <c r="M61" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>DigiKey</v>
       </c>
       <c r="N61" s="50">
@@ -5647,14 +5647,14 @@
         <v>2</v>
       </c>
       <c r="P61" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.4</v>
       </c>
       <c r="Q61" s="33"/>
       <c r="R61" s="25"/>
       <c r="S61" s="8"/>
       <c r="U61">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -5684,7 +5684,7 @@
         <v>36</v>
       </c>
       <c r="M62" s="48" t="str">
-        <f t="shared" ref="M62:M68" si="16">HYPERLINK(L62,J62)</f>
+        <f t="shared" ref="M62:M68" si="19">HYPERLINK(L62,J62)</f>
         <v>DigiKey</v>
       </c>
       <c r="N62" s="50">
@@ -5694,7 +5694,7 @@
         <v>8</v>
       </c>
       <c r="P62" s="32">
-        <f t="shared" ref="P62:P68" si="17">N62*O62</f>
+        <f t="shared" ref="P62:P67" si="20">N62*O62</f>
         <v>7.04</v>
       </c>
       <c r="Q62" s="33" t="s">
@@ -5709,7 +5709,7 @@
         <v>7.04</v>
       </c>
       <c r="U62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AF62" t="s">
@@ -5745,7 +5745,7 @@
         <v>356</v>
       </c>
       <c r="M63" s="48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>DigiKey</v>
       </c>
       <c r="N63" s="50">
@@ -5755,14 +5755,14 @@
         <v>4</v>
       </c>
       <c r="P63" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="Q63" s="33"/>
       <c r="R63" s="25"/>
       <c r="S63" s="6"/>
       <c r="U63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -5794,7 +5794,7 @@
         <v>40</v>
       </c>
       <c r="M64" s="48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>DigiKey</v>
       </c>
       <c r="N64" s="50">
@@ -5804,7 +5804,7 @@
         <v>4</v>
       </c>
       <c r="P64" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2.2799999999999998</v>
       </c>
       <c r="Q64" s="30" t="s">
@@ -5851,7 +5851,7 @@
         <v>43</v>
       </c>
       <c r="M65" s="48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>DigiKey</v>
       </c>
       <c r="N65" s="50">
@@ -5861,7 +5861,7 @@
         <v>4</v>
       </c>
       <c r="P65" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="Q65" s="33" t="s">
@@ -5910,7 +5910,7 @@
         <v>274</v>
       </c>
       <c r="M66" s="48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>DigiKey</v>
       </c>
       <c r="N66" s="50">
@@ -5920,14 +5920,14 @@
         <v>2</v>
       </c>
       <c r="P66" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5.2</v>
       </c>
       <c r="Q66" s="33"/>
       <c r="R66" s="25"/>
       <c r="S66" s="6"/>
       <c r="U66">
-        <f t="shared" ref="U66:U68" si="18">SUBTOTAL(103, G66)</f>
+        <f t="shared" ref="U66:U68" si="21">SUBTOTAL(103, G66)</f>
         <v>0</v>
       </c>
       <c r="AF66" t="s">
@@ -5967,7 +5967,7 @@
         <v>276</v>
       </c>
       <c r="M67" s="48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>DigiKey</v>
       </c>
       <c r="N67" s="50">
@@ -5977,14 +5977,14 @@
         <v>1</v>
       </c>
       <c r="P67" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>1.53</v>
       </c>
       <c r="Q67" s="33"/>
       <c r="R67" s="25"/>
       <c r="S67" s="6"/>
       <c r="U67">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AF67" t="s">
@@ -6024,7 +6024,7 @@
         <v>348</v>
       </c>
       <c r="M68" s="48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>Mouser</v>
       </c>
       <c r="N68" s="50">
@@ -6041,7 +6041,7 @@
       <c r="R68" s="25"/>
       <c r="S68" s="6"/>
       <c r="U68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AF68" t="s">
@@ -6079,7 +6079,7 @@
         <v>50</v>
       </c>
       <c r="M69" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Amazon</v>
       </c>
       <c r="N69" s="50">
@@ -6089,7 +6089,7 @@
         <v>1</v>
       </c>
       <c r="P69" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.66</v>
       </c>
       <c r="Q69" s="33" t="s">
@@ -6135,7 +6135,7 @@
         <v>210</v>
       </c>
       <c r="M70" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Amazon</v>
       </c>
       <c r="N70" s="50">
@@ -6145,7 +6145,7 @@
         <v>1</v>
       </c>
       <c r="P70" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.99</v>
       </c>
       <c r="Q70" s="30" t="s">
@@ -6191,7 +6191,7 @@
         <v>210</v>
       </c>
       <c r="M71" s="48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Amazon</v>
       </c>
       <c r="N71" s="50">
@@ -6201,7 +6201,7 @@
         <v>1</v>
       </c>
       <c r="P71" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>18.14</v>
       </c>
       <c r="Q71" s="33" t="s">
@@ -6460,108 +6460,12 @@
     </filterColumn>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{2376F375-2D91-4AB8-9819-CC132C3118EA}" filter="1" showAutoFilter="1" hiddenRows="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P68" sqref="B1:P68"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:R71" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BL"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="Lk2"/>
-            <filter val="POW2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="ST_TEMP"/>
-            <filter val="ST3"/>
-            <filter val="SV2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{1253E34A-3A91-496E-8486-95C1D21A2085}" showAutoFilter="1" hiddenColumns="1" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE10" sqref="AE10"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:R76" xr:uid="{7E256883-3769-4722-82A9-5D03FDA1740C}"/>
-    </customSheetView>
-    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A1:R59" xr:uid="{C448D155-4C6D-4265-A8BD-4B52118AED66}"/>
-    </customSheetView>
-    <customSheetView guid="{3411E606-57DF-4B4E-942D-8A879EBC3FAD}" filter="1" showAutoFilter="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A1:R76" xr:uid="{7A2D0453-9AA5-453F-A4D5-E6C6A702F732}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BL"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="Lk2"/>
-            <filter val="POW2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="ST_TEMP"/>
-            <filter val="ST3"/>
-            <filter val="SV2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{0C0F82AC-DC21-4B4A-94AC-E96E30BF52DE}" filter="1" showAutoFilter="1" hiddenRows="1" hiddenColumns="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P79" sqref="P79"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-      <autoFilter ref="A1:R76" xr:uid="{DDFFDB25-097D-4B4C-95C6-1C8921FE262A}">
-        <filterColumn colId="0">
-          <filters blank="1">
-            <filter val="ACC3"/>
-            <filter val="BF4"/>
-            <filter val="BL"/>
-            <filter val="BP2"/>
-            <filter val="F2"/>
-            <filter val="Lk2"/>
-            <filter val="POW2"/>
-            <filter val="S1"/>
-            <filter val="SP2"/>
-            <filter val="ST_TEMP"/>
-            <filter val="ST3"/>
-            <filter val="SV2"/>
-            <filter val="TP2"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{4300A442-0A40-4FB1-A9F3-2AB99D5A4993}" showAutoFilter="1" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-      <autoFilter ref="A1:R76" xr:uid="{9D24E325-D76E-480F-8644-7C22A41F4F8F}"/>
-    </customSheetView>
     <customSheetView guid="{E35F6895-3697-4266-BC90-C5022F400E13}" filter="1" showAutoFilter="1" hiddenRows="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O83" sqref="B1:O83"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
-      <autoFilter ref="A1:R76" xr:uid="{3AA576F5-B598-4ECC-B3D6-C7907F3D5042}">
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:R76" xr:uid="{CB1EAF7E-02F6-4D5D-A76F-EFD137539F9A}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6586,6 +6490,102 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
+    <customSheetView guid="{4300A442-0A40-4FB1-A9F3-2AB99D5A4993}" showAutoFilter="1" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A1:R76" xr:uid="{9A0E93AC-43CE-433C-A2DE-012A08E823D2}"/>
+    </customSheetView>
+    <customSheetView guid="{0C0F82AC-DC21-4B4A-94AC-E96E30BF52DE}" filter="1" showAutoFilter="1" hiddenRows="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P79" sqref="P79"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A1:R76" xr:uid="{72645865-D38B-4F6F-A7D0-55DE811D6FB0}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BL"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="Lk2"/>
+            <filter val="POW2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="ST_TEMP"/>
+            <filter val="ST3"/>
+            <filter val="SV2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{3411E606-57DF-4B4E-942D-8A879EBC3FAD}" filter="1" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <autoFilter ref="A1:R76" xr:uid="{2E3A0D1C-5AE9-4788-A882-A5901F38DA7D}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BL"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="Lk2"/>
+            <filter val="POW2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="ST_TEMP"/>
+            <filter val="ST3"/>
+            <filter val="SV2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{14407C96-79A3-4D80-86DC-7BE14F8182CE}" showAutoFilter="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+      <autoFilter ref="A1:R59" xr:uid="{1AC29075-00DC-42F3-B03E-0093CB69CEB7}"/>
+    </customSheetView>
+    <customSheetView guid="{1253E34A-3A91-496E-8486-95C1D21A2085}" showAutoFilter="1" hiddenColumns="1" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE10" sqref="AE10"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+      <autoFilter ref="A1:R76" xr:uid="{3658F8ED-602E-4E83-AE47-F02C98024198}"/>
+    </customSheetView>
+    <customSheetView guid="{2376F375-2D91-4AB8-9819-CC132C3118EA}" filter="1" showAutoFilter="1" hiddenRows="1" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P68" sqref="B1:P68"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+      <autoFilter ref="A1:R71" xr:uid="{1A5BA1EF-1420-4CBE-847F-720606E6B9EC}">
+        <filterColumn colId="0">
+          <filters blank="1">
+            <filter val="ACC3"/>
+            <filter val="BF4"/>
+            <filter val="BL"/>
+            <filter val="BP2"/>
+            <filter val="F2"/>
+            <filter val="Lk2"/>
+            <filter val="POW2"/>
+            <filter val="S1"/>
+            <filter val="SP2"/>
+            <filter val="ST_TEMP"/>
+            <filter val="ST3"/>
+            <filter val="SV2"/>
+            <filter val="TP2"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="4">
     <mergeCell ref="AB1:AC1"/>
@@ -6606,7 +6606,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q79:Q1048576 Q1:Q77">
+  <conditionalFormatting sqref="Q1:Q77 Q79:Q1048576">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Nicht Gekauft"</formula>
     </cfRule>

</xml_diff>

<commit_message>
cleanup, want to get the workflow running soon in the future
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
+++ b/2nd_mainboard_bom/elektronik_gespeicherte_Filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F960C3C-67C3-492C-A72B-95E82004F3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341F2E70-C3C1-46FF-AF14-38DF4D5FABFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2402,7 +2402,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z36" sqref="Z36"/>
+      <selection pane="bottomLeft" activeCell="AI25" sqref="AI25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6465,7 +6465,7 @@
       <selection pane="bottomLeft" activeCell="O83" sqref="B1:O83"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:R76" xr:uid="{CB1EAF7E-02F6-4D5D-A76F-EFD137539F9A}">
+      <autoFilter ref="A1:R76" xr:uid="{3114BF07-23E2-4524-8606-01F5F3BB4E60}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6495,14 +6495,14 @@
       <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:R76" xr:uid="{9A0E93AC-43CE-433C-A2DE-012A08E823D2}"/>
+      <autoFilter ref="A1:R76" xr:uid="{DAFBC8F6-BDD0-4E20-BDF2-9FC45711A5A7}"/>
     </customSheetView>
     <customSheetView guid="{0C0F82AC-DC21-4B4A-94AC-E96E30BF52DE}" filter="1" showAutoFilter="1" hiddenRows="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P79" sqref="P79"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A1:R76" xr:uid="{72645865-D38B-4F6F-A7D0-55DE811D6FB0}">
+      <autoFilter ref="A1:R76" xr:uid="{20AE68FC-6621-47B4-BAA3-516505CDD435}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6527,7 +6527,7 @@
       <selection pane="bottomLeft" activeCell="X29" sqref="X29"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A1:R76" xr:uid="{2E3A0D1C-5AE9-4788-A882-A5901F38DA7D}">
+      <autoFilter ref="A1:R76" xr:uid="{96C9180D-D978-49DC-A2E3-B7F24EF3C2FC}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>
@@ -6552,21 +6552,21 @@
       <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-      <autoFilter ref="A1:R59" xr:uid="{1AC29075-00DC-42F3-B03E-0093CB69CEB7}"/>
+      <autoFilter ref="A1:R59" xr:uid="{0573B8B4-DF71-49AC-9D33-1CACBE998FCA}"/>
     </customSheetView>
     <customSheetView guid="{1253E34A-3A91-496E-8486-95C1D21A2085}" showAutoFilter="1" hiddenColumns="1" topLeftCell="B1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AE10" sqref="AE10"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-      <autoFilter ref="A1:R76" xr:uid="{3658F8ED-602E-4E83-AE47-F02C98024198}"/>
+      <autoFilter ref="A1:R76" xr:uid="{C22459C7-1C41-4D59-997A-EE78C1EC479B}"/>
     </customSheetView>
     <customSheetView guid="{2376F375-2D91-4AB8-9819-CC132C3118EA}" filter="1" showAutoFilter="1" hiddenRows="1" hiddenColumns="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P68" sqref="B1:P68"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
-      <autoFilter ref="A1:R71" xr:uid="{1A5BA1EF-1420-4CBE-847F-720606E6B9EC}">
+      <autoFilter ref="A1:R71" xr:uid="{B20E23BA-EF5C-4BCE-A577-E4469C0454F1}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="ACC3"/>

</xml_diff>